<commit_message>
Repare scenarios section + add diagrams
</commit_message>
<xml_diff>
--- a/excel-use-cases/MAESHA/IEC62559-2_TEMPLATE_FrequencyControlUC.xlsx
+++ b/excel-use-cases/MAESHA/IEC62559-2_TEMPLATE_FrequencyControlUC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MAESHA\08_BRIDGE\Data Management WG\UC repository\MAESHA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B47C550-3B15-4C42-9297-8EE7E48B67FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAF5768-059A-4AA1-831F-5AE119D9538A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IEC62559-2" sheetId="1" r:id="rId1"/>
@@ -1363,7 +1363,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="595">
   <si>
     <t>1 Description of the use case</t>
   </si>
@@ -1680,37 +1680,19 @@
     <t>Image</t>
   </si>
   <si>
-    <t>BusinessLayer_FrequencyControlUC</t>
-  </si>
-  <si>
     <t>SGAM Function layer of the frequency control use case-specific architecture</t>
   </si>
   <si>
-    <t>FunctionLayer_FrequencyControlUC</t>
-  </si>
-  <si>
     <t>Overview of phases of frequency control after a major outage</t>
   </si>
   <si>
-    <t>FrequencyControlPhasesAfterMajorOutage</t>
-  </si>
-  <si>
     <t>FCR achitecture overview</t>
   </si>
   <si>
-    <t>FCR_Architecture</t>
-  </si>
-  <si>
     <t>FRR achitecture overview</t>
   </si>
   <si>
-    <t>FRR_Architecture</t>
-  </si>
-  <si>
     <t>Architecture overview for frequency control in MAESHA</t>
-  </si>
-  <si>
-    <t>FrequencyControlArchi_OverviewMAESHA</t>
   </si>
   <si>
     <t>Business Actor</t>
@@ -1938,21 +1920,12 @@
     <t>Calculating the amount of FCR and FRR needed</t>
   </si>
   <si>
-    <t>System Operator</t>
-  </si>
-  <si>
     <t>Long-term planning (yearly activity)</t>
   </si>
   <si>
     <t>Required amount of Inertia, FCR, FRR to be contracted and reserved are defined</t>
   </si>
   <si>
-    <t>Need for: 
-- Historic data about electricity system
-- Mid-term consumption forecasts
-- List of planned new DER installations</t>
-  </si>
-  <si>
     <t>Sc2</t>
   </si>
   <si>
@@ -1980,9 +1953,6 @@
     <t>Detection of the frequency deviations centrally in the SCADA</t>
   </si>
   <si>
-    <t>System Operator, with the help of the AGC</t>
-  </si>
-  <si>
     <t>Frequency deviations are detected by central AGC</t>
   </si>
   <si>
@@ -2079,12 +2049,6 @@
     <t>Flexibility bid is accepted via FMTP</t>
   </si>
   <si>
-    <t>Sc1 - Frequency reserve requirements</t>
-  </si>
-  <si>
-    <t>St1</t>
-  </si>
-  <si>
     <t>Periodically (yearly)</t>
   </si>
   <si>
@@ -2101,9 +2065,6 @@
   </si>
   <si>
     <t>R-01-01 (guidelines for operation defined by regulator)</t>
-  </si>
-  <si>
-    <t>St2</t>
   </si>
   <si>
     <t>Collect data of the power system</t>
@@ -2123,9 +2084,6 @@
     <t>R-01-02 (historic data about electricity system, load and frequency)</t>
   </si>
   <si>
-    <t xml:space="preserve">St3 </t>
-  </si>
-  <si>
     <t>Mid-term &amp; long-term forecasts</t>
   </si>
   <si>
@@ -2138,9 +2096,6 @@
     <t>R-01-03 (List of planned new DER installations)</t>
   </si>
   <si>
-    <t>St4</t>
-  </si>
-  <si>
     <t>Define design scenarios</t>
   </si>
   <si>
@@ -2153,9 +2108,6 @@
     <t>IE-01, IE-02, IE-03, IE-04, IE-05 received</t>
   </si>
   <si>
-    <t>St5</t>
-  </si>
-  <si>
     <t>Calculate the required amount of flexibility- balancing reserve needed on the island - FRR</t>
   </si>
   <si>
@@ -2168,9 +2120,6 @@
     <t>IE-01, IE-02, IE-03, IE-04, IE-05, IE-06 received</t>
   </si>
   <si>
-    <t>St6</t>
-  </si>
-  <si>
     <t>St5 finished</t>
   </si>
   <si>
@@ -2186,9 +2135,6 @@
     <t>IE-01-07 received</t>
   </si>
   <si>
-    <t>Sc2 - Detection of the frequency issues - Frequency Containment Reservce (FCR)</t>
-  </si>
-  <si>
     <t>Periodically (interval of 1s of faster)</t>
   </si>
   <si>
@@ -2204,9 +2150,6 @@
     <t>R-02-01 (frequency meter on-site)</t>
   </si>
   <si>
-    <t>St3</t>
-  </si>
-  <si>
     <t>New frequency measurement available</t>
   </si>
   <si>
@@ -2234,9 +2177,6 @@
     <t>IE-02-02 (frequency deviation)</t>
   </si>
   <si>
-    <t>Sc3 - Detection of the frequency issues - Frequency Restoration Reserve (FRR)</t>
-  </si>
-  <si>
     <t>Continuously</t>
   </si>
   <si>
@@ -2303,9 +2243,6 @@
     <t>R-03-04 (P-f- control algorithm)</t>
   </si>
   <si>
-    <t>Sc4 - Contracting balancing service products</t>
-  </si>
-  <si>
     <t xml:space="preserve">After definition of technical require-ments </t>
   </si>
   <si>
@@ -2405,9 +2342,6 @@
     <t>IE-04-05, R-04-01 (prequalified flexibility providers)</t>
   </si>
   <si>
-    <t>St7</t>
-  </si>
-  <si>
     <t>SO received bid for balancing service provision</t>
   </si>
   <si>
@@ -2421,9 +2355,6 @@
   </si>
   <si>
     <t>IE-04-06 received</t>
-  </si>
-  <si>
-    <t>Sc5 - Flexibility activation through local controller - FCR</t>
   </si>
   <si>
     <t>Reception of FCR bid acceptance</t>
@@ -2521,9 +2452,6 @@
     <t>The flexibility provider updates the DER control algorithms in order to remedy the FCR malperformance and to provide the FCR service according to technical specifications.</t>
   </si>
   <si>
-    <t>Sc6 - Flexibility activation through the Flexibility Management and Trading Platform - FRR</t>
-  </si>
-  <si>
     <t>Reception of FRR bid acceptance</t>
   </si>
   <si>
@@ -2576,12 +2504,6 @@
     <t>R-06-02 (central balancing asset available)</t>
   </si>
   <si>
-    <t>St3a</t>
-  </si>
-  <si>
-    <t>St3b</t>
-  </si>
-  <si>
     <t>Decentral assets’ FRR setpoint updated</t>
   </si>
   <si>
@@ -2658,9 +2580,6 @@
 R-05-05 (active power meter, on-site)</t>
   </si>
   <si>
-    <t>St8</t>
-  </si>
-  <si>
     <t>Send monitoring data to AGC</t>
   </si>
   <si>
@@ -2674,12 +2593,6 @@
     <t>R-06-06 (communication channel between FMTP and intermediate platforms or large DER)</t>
   </si>
   <si>
-    <t>St9</t>
-  </si>
-  <si>
-    <t>St9a</t>
-  </si>
-  <si>
     <t>Validate FRR provision</t>
   </si>
   <si>
@@ -2692,9 +2605,6 @@
     <t>R-06-08 (algorithm to validate FRR performance)</t>
   </si>
   <si>
-    <t>St9b</t>
-  </si>
-  <si>
     <t>Yearly</t>
   </si>
   <si>
@@ -2704,18 +2614,12 @@
     <t>R-06-09 (meter data)</t>
   </si>
   <si>
-    <t>St10</t>
-  </si>
-  <si>
     <t>FRR malperformance detected</t>
   </si>
   <si>
     <t>The SO informs the flexibility provider about the FRR malperformance and orders immediate correction of the behaviour.</t>
   </si>
   <si>
-    <t>St11</t>
-  </si>
-  <si>
     <t>FRR validation report received</t>
   </si>
   <si>
@@ -2723,9 +2627,6 @@
   </si>
   <si>
     <t>The flexibility provider updates the DER control algorithms in order to remedy the FRR malperformance and to provide the FRR service according to technical specifications.</t>
-  </si>
-  <si>
-    <t>Sc7-Settlement process to remunerate flexibility activation</t>
   </si>
   <si>
     <t>Daily</t>
@@ -2769,9 +2670,6 @@
     <t>IE-07-02 (monthly balancing service accounting and remuneration report)</t>
   </si>
   <si>
-    <t>Sc8-Frequency control by flexibility provider</t>
-  </si>
-  <si>
     <t xml:space="preserve">Forecast flexible capacity for upcoming tender period </t>
   </si>
   <si>
@@ -2879,9 +2777,6 @@
     <t>The PLC receives a setpoint of 0 MW to end the ongoing activation.</t>
   </si>
   <si>
-    <t>St12</t>
-  </si>
-  <si>
     <t>Activation end received by DER</t>
   </si>
   <si>
@@ -2889,9 +2784,6 @@
   </si>
   <si>
     <t>The PLC of the DER initiates the end activation program (ramp-down) in order and the balancing energy provision within the FAT.</t>
-  </si>
-  <si>
-    <t>St13</t>
   </si>
   <si>
     <t>Continuously (e.g., 2s interval)</t>
@@ -3564,6 +3456,51 @@
   </si>
   <si>
     <t>Aggregated monitoring data of a pool of DER (managed by an intermediary platform), which is sent to the FMTP. Datapoints: active power, baseline, setpoint, FRR activation, control bandwidth</t>
+  </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>9a</t>
+  </si>
+  <si>
+    <t>9b</t>
+  </si>
+  <si>
+    <t>Detection of the frequency issues - Frequency Containment Reservce (FCR)</t>
+  </si>
+  <si>
+    <t>Detection of the frequency issues - Frequency Restoration Reserve (FRR)</t>
+  </si>
+  <si>
+    <t>Flexibility activation through the Flexibility Management and Trading Platform - FRR</t>
+  </si>
+  <si>
+    <t>TSO, AGC</t>
+  </si>
+  <si>
+    <t>Need for historical data about electricity system, mid-term consumption forecasts and list of planned new DER installations</t>
+  </si>
+  <si>
+    <t>BusinessLayer_FrequencyControlUC.png</t>
+  </si>
+  <si>
+    <t>FunctionLayer_FrequencyControlUC.png</t>
+  </si>
+  <si>
+    <t>FrequencyControlPhasesAfterMajorOutage.png</t>
+  </si>
+  <si>
+    <t>FCR_Architecture.png</t>
+  </si>
+  <si>
+    <t>FRR_Architecture.png</t>
+  </si>
+  <si>
+    <t>FrequencyControlArchi_OverviewMAESHA.png</t>
   </si>
 </sst>
 </file>
@@ -4306,8 +4243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC79" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG87" sqref="AG87"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4412,7 +4349,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>609</v>
+        <v>574</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -4508,7 +4445,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="58" x14ac:dyDescent="0.35">
@@ -4542,7 +4479,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
@@ -4551,7 +4488,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>610</v>
+        <v>575</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -4628,7 +4565,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>611</v>
+        <v>576</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -4640,7 +4577,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>612</v>
+        <v>577</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="19"/>
@@ -4752,19 +4689,19 @@
         <v>102</v>
       </c>
       <c r="D38" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="F38" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="F38" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="G38" s="18" t="s">
-        <v>112</v>
-      </c>
       <c r="H38" s="18" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:22" x14ac:dyDescent="0.35">
@@ -4820,22 +4757,22 @@
         <v>80</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>105</v>
+        <v>589</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>107</v>
+        <v>590</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>109</v>
+        <v>591</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>111</v>
+        <v>592</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>113</v>
+        <v>593</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>115</v>
+        <v>594</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4876,16 +4813,16 @@
         <v>39</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
@@ -4910,10 +4847,10 @@
         <v>40</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
@@ -4940,64 +4877,64 @@
         <v>41</v>
       </c>
       <c r="C46" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D46" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="E46" s="18" t="s">
-        <v>128</v>
-      </c>
       <c r="F46" s="18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G46" s="18" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H46" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="I46" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="J46" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="K46" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="I46" s="18" t="s">
+      <c r="L46" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="J46" s="18" t="s">
+      <c r="M46" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="K46" s="18" t="s">
+      <c r="N46" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="L46" s="18" t="s">
-        <v>143</v>
-      </c>
-      <c r="M46" s="18" t="s">
+      <c r="O46" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="N46" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="O46" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="P46" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q46" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="R46" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="S46" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="Q46" s="18" t="s">
+      <c r="T46" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="R46" s="18" t="s">
+      <c r="U46" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="V46" s="18" t="s">
         <v>156</v>
-      </c>
-      <c r="S46" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="T46" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="U46" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="V46" s="18" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:22" x14ac:dyDescent="0.35">
@@ -5006,64 +4943,64 @@
         <v>42</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="I47" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J47" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="K47" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="M47" s="18" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="N47" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="O47" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="P47" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="Q47" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="R47" s="18" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="S47" s="18" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="T47" s="18" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="U47" s="18" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="V47" s="18" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:22" ht="58" x14ac:dyDescent="0.35">
@@ -5072,62 +5009,62 @@
         <v>43</v>
       </c>
       <c r="C48" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="E48" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="D48" s="26" t="s">
-        <v>127</v>
-      </c>
-      <c r="E48" s="18" t="s">
-        <v>129</v>
-      </c>
       <c r="F48" s="26" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G48" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="H48" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="I48" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="J48" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="H48" s="26" t="s">
+      <c r="K48" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="I48" s="26" t="s">
+      <c r="L48" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="J48" s="26" t="s">
+      <c r="M48" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="K48" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="L48" s="26" t="s">
+      <c r="N48" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="O48" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="M48" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="N48" s="26" t="s">
+      <c r="P48" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q48" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="O48" s="26" t="s">
-        <v>150</v>
-      </c>
-      <c r="P48" s="26" t="s">
-        <v>153</v>
-      </c>
-      <c r="Q48" s="26" t="s">
-        <v>155</v>
-      </c>
       <c r="R48" s="26" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="S48" s="26"/>
       <c r="T48" s="26" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="U48" s="26" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="V48" s="26" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:22" x14ac:dyDescent="0.35">
@@ -5136,7 +5073,7 @@
         <v>44</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
@@ -5174,13 +5111,13 @@
         <v>21</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D51" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="E51" s="18" t="s">
         <v>175</v>
-      </c>
-      <c r="E51" s="18" t="s">
-        <v>181</v>
       </c>
       <c r="F51" s="18"/>
     </row>
@@ -5190,13 +5127,13 @@
         <v>46</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D52" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>176</v>
-      </c>
-      <c r="E52" s="18" t="s">
-        <v>182</v>
       </c>
       <c r="F52" s="18"/>
     </row>
@@ -5206,13 +5143,13 @@
         <v>47</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F53" s="18"/>
     </row>
@@ -5222,13 +5159,13 @@
         <v>48</v>
       </c>
       <c r="C54" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="D54" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="D54" s="18" t="s">
-        <v>177</v>
-      </c>
       <c r="E54" s="18" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F54" s="18"/>
     </row>
@@ -5244,7 +5181,7 @@
         <v>90</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="F55" s="18"/>
     </row>
@@ -5254,13 +5191,13 @@
         <v>50</v>
       </c>
       <c r="C56" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="D56" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="D56" s="18" t="s">
-        <v>178</v>
-      </c>
       <c r="E56" s="18" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F56" s="18"/>
     </row>
@@ -5270,13 +5207,13 @@
         <v>51</v>
       </c>
       <c r="C57" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D57" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="D57" s="18" t="s">
-        <v>179</v>
-      </c>
       <c r="E57" s="18" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F57" s="18"/>
     </row>
@@ -5286,13 +5223,13 @@
         <v>52</v>
       </c>
       <c r="C58" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" s="28" t="s">
         <v>174</v>
       </c>
-      <c r="D58" s="28" t="s">
+      <c r="E58" s="29" t="s">
         <v>180</v>
-      </c>
-      <c r="E58" s="29" t="s">
-        <v>186</v>
       </c>
       <c r="F58" s="18"/>
     </row>
@@ -5330,28 +5267,28 @@
         <v>46</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="I62" s="18" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="J62" s="18" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:22" ht="29" x14ac:dyDescent="0.35">
@@ -5360,28 +5297,28 @@
         <v>56</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F63" s="18" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="H63" s="26" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="I63" s="26" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="J63" s="26" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="64" spans="1:22" ht="29" x14ac:dyDescent="0.35">
@@ -5390,28 +5327,28 @@
         <v>57</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D64" s="26" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="F64" s="26" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="G64" s="26" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="H64" s="26" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="I64" s="26" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="J64" s="26" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="65" spans="1:59" x14ac:dyDescent="0.35">
@@ -5420,28 +5357,28 @@
         <v>58</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>203</v>
+        <v>587</v>
       </c>
       <c r="F65" s="18" t="s">
-        <v>190</v>
+        <v>116</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="I65" s="18" t="s">
-        <v>226</v>
+        <v>116</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:59" x14ac:dyDescent="0.35">
@@ -5450,58 +5387,58 @@
         <v>59</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="67" spans="1:59" ht="58" x14ac:dyDescent="0.35">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="67" spans="1:59" ht="29" x14ac:dyDescent="0.35">
       <c r="A67" s="3"/>
       <c r="B67" s="15" t="s">
         <v>60</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>193</v>
+        <v>588</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F67" s="18" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="H67" s="26" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="I67" s="26" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="J67" s="26" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="68" spans="1:59" ht="29" x14ac:dyDescent="0.35">
@@ -5510,28 +5447,28 @@
         <v>61</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="G68" s="26" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="H68" s="26" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="I68" s="26" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="J68" s="26" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="69" spans="1:59" x14ac:dyDescent="0.35">
@@ -5603,175 +5540,175 @@
         <v>63</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>236</v>
+        <v>182</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>236</v>
+        <v>182</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>236</v>
+        <v>182</v>
       </c>
       <c r="F70" s="18" t="s">
-        <v>236</v>
+        <v>182</v>
       </c>
       <c r="G70" s="18" t="s">
-        <v>236</v>
+        <v>182</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>236</v>
+        <v>182</v>
       </c>
       <c r="I70" s="26" t="s">
-        <v>271</v>
+        <v>584</v>
       </c>
       <c r="J70" s="26" t="s">
-        <v>271</v>
+        <v>584</v>
       </c>
       <c r="K70" s="26" t="s">
-        <v>271</v>
+        <v>584</v>
       </c>
       <c r="L70" s="26" t="s">
-        <v>287</v>
+        <v>585</v>
       </c>
       <c r="M70" s="26" t="s">
-        <v>287</v>
+        <v>585</v>
       </c>
       <c r="N70" s="26" t="s">
-        <v>287</v>
+        <v>585</v>
       </c>
       <c r="O70" s="26" t="s">
-        <v>287</v>
+        <v>585</v>
       </c>
       <c r="P70" s="26" t="s">
-        <v>287</v>
+        <v>585</v>
       </c>
       <c r="Q70" s="26" t="s">
-        <v>310</v>
+        <v>197</v>
       </c>
       <c r="R70" s="26" t="s">
-        <v>310</v>
+        <v>197</v>
       </c>
       <c r="S70" s="26" t="s">
-        <v>310</v>
+        <v>197</v>
       </c>
       <c r="T70" s="26" t="s">
-        <v>310</v>
+        <v>197</v>
       </c>
       <c r="U70" s="26" t="s">
-        <v>310</v>
+        <v>197</v>
       </c>
       <c r="V70" s="26" t="s">
-        <v>310</v>
+        <v>197</v>
       </c>
       <c r="W70" s="26" t="s">
-        <v>310</v>
+        <v>197</v>
       </c>
       <c r="X70" s="26" t="s">
-        <v>350</v>
+        <v>203</v>
       </c>
       <c r="Y70" s="26" t="s">
-        <v>350</v>
+        <v>203</v>
       </c>
       <c r="Z70" s="26" t="s">
-        <v>350</v>
+        <v>203</v>
       </c>
       <c r="AA70" s="26" t="s">
-        <v>350</v>
+        <v>203</v>
       </c>
       <c r="AB70" s="26" t="s">
-        <v>350</v>
+        <v>203</v>
       </c>
       <c r="AC70" s="26" t="s">
-        <v>350</v>
+        <v>203</v>
       </c>
       <c r="AD70" s="26" t="s">
-        <v>350</v>
+        <v>203</v>
       </c>
       <c r="AE70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AF70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AG70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AH70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AI70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AJ70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AK70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AL70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AM70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AN70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AO70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AP70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AQ70" s="26" t="s">
-        <v>382</v>
+        <v>586</v>
       </c>
       <c r="AR70" s="26" t="s">
-        <v>448</v>
+        <v>215</v>
       </c>
       <c r="AS70" s="26" t="s">
-        <v>448</v>
+        <v>215</v>
       </c>
       <c r="AT70" s="26" t="s">
-        <v>448</v>
+        <v>215</v>
       </c>
       <c r="AU70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="AV70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="AW70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="AX70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="AY70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="AZ70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="BA70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="BB70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="BC70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="BD70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="BE70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="BF70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
       <c r="BG70" s="26" t="s">
-        <v>462</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" spans="1:59" x14ac:dyDescent="0.35">
@@ -5779,176 +5716,176 @@
       <c r="B71" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C71" s="7" t="s">
-        <v>237</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="E71" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="F71" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="G71" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="H71" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="I71" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="J71" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="K71" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="L71" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="M71" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="N71" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="O71" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="P71" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q71" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="R71" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="S71" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="T71" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="U71" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="V71" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="W71" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="X71" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y71" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="Z71" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="AA71" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="AB71" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="AC71" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="AD71" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="AE71" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="AF71" s="18" t="s">
-        <v>244</v>
+      <c r="C71" s="7">
+        <v>1</v>
+      </c>
+      <c r="D71" s="18">
+        <v>2</v>
+      </c>
+      <c r="E71" s="18">
+        <v>3</v>
+      </c>
+      <c r="F71" s="18">
+        <v>4</v>
+      </c>
+      <c r="G71" s="18">
+        <v>5</v>
+      </c>
+      <c r="H71" s="18">
+        <v>6</v>
+      </c>
+      <c r="I71" s="18">
+        <v>1</v>
+      </c>
+      <c r="J71" s="18">
+        <v>2</v>
+      </c>
+      <c r="K71" s="18">
+        <v>3</v>
+      </c>
+      <c r="L71" s="18">
+        <v>1</v>
+      </c>
+      <c r="M71" s="18">
+        <v>2</v>
+      </c>
+      <c r="N71" s="18">
+        <v>3</v>
+      </c>
+      <c r="O71" s="18">
+        <v>4</v>
+      </c>
+      <c r="P71" s="18">
+        <v>5</v>
+      </c>
+      <c r="Q71" s="18">
+        <v>1</v>
+      </c>
+      <c r="R71" s="18">
+        <v>2</v>
+      </c>
+      <c r="S71" s="18">
+        <v>3</v>
+      </c>
+      <c r="T71" s="18">
+        <v>4</v>
+      </c>
+      <c r="U71" s="18">
+        <v>5</v>
+      </c>
+      <c r="V71" s="18">
+        <v>6</v>
+      </c>
+      <c r="W71" s="18">
+        <v>7</v>
+      </c>
+      <c r="X71" s="18">
+        <v>1</v>
+      </c>
+      <c r="Y71" s="18">
+        <v>2</v>
+      </c>
+      <c r="Z71" s="18">
+        <v>3</v>
+      </c>
+      <c r="AA71" s="18">
+        <v>4</v>
+      </c>
+      <c r="AB71" s="18">
+        <v>5</v>
+      </c>
+      <c r="AC71" s="18">
+        <v>6</v>
+      </c>
+      <c r="AD71" s="18">
+        <v>7</v>
+      </c>
+      <c r="AE71" s="18">
+        <v>1</v>
+      </c>
+      <c r="AF71" s="18">
+        <v>2</v>
       </c>
       <c r="AG71" s="18" t="s">
-        <v>400</v>
+        <v>580</v>
       </c>
       <c r="AH71" s="18" t="s">
-        <v>401</v>
-      </c>
-      <c r="AI71" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="AJ71" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="AK71" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="AL71" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="AM71" s="18" t="s">
-        <v>426</v>
+        <v>581</v>
+      </c>
+      <c r="AI71" s="18">
+        <v>4</v>
+      </c>
+      <c r="AJ71" s="18">
+        <v>5</v>
+      </c>
+      <c r="AK71" s="18">
+        <v>6</v>
+      </c>
+      <c r="AL71" s="18">
+        <v>7</v>
+      </c>
+      <c r="AM71" s="18">
+        <v>8</v>
       </c>
       <c r="AN71" s="18" t="s">
-        <v>432</v>
+        <v>582</v>
       </c>
       <c r="AO71" s="18" t="s">
-        <v>437</v>
-      </c>
-      <c r="AP71" s="18" t="s">
-        <v>441</v>
-      </c>
-      <c r="AQ71" s="18" t="s">
-        <v>444</v>
-      </c>
-      <c r="AR71" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="AS71" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="AT71" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="AU71" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="AV71" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="AW71" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="AX71" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="AY71" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="AZ71" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="BA71" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="BB71" s="18" t="s">
-        <v>426</v>
-      </c>
-      <c r="BC71" s="18" t="s">
-        <v>431</v>
-      </c>
-      <c r="BD71" s="18" t="s">
-        <v>441</v>
-      </c>
-      <c r="BE71" s="18" t="s">
-        <v>444</v>
-      </c>
-      <c r="BF71" s="18" t="s">
-        <v>498</v>
-      </c>
-      <c r="BG71" s="18" t="s">
-        <v>502</v>
+        <v>583</v>
+      </c>
+      <c r="AP71" s="18">
+        <v>10</v>
+      </c>
+      <c r="AQ71" s="18">
+        <v>11</v>
+      </c>
+      <c r="AR71" s="18">
+        <v>1</v>
+      </c>
+      <c r="AS71" s="18">
+        <v>2</v>
+      </c>
+      <c r="AT71" s="18">
+        <v>3</v>
+      </c>
+      <c r="AU71" s="18">
+        <v>1</v>
+      </c>
+      <c r="AV71" s="18">
+        <v>2</v>
+      </c>
+      <c r="AW71" s="18">
+        <v>3</v>
+      </c>
+      <c r="AX71" s="18">
+        <v>4</v>
+      </c>
+      <c r="AY71" s="18">
+        <v>5</v>
+      </c>
+      <c r="AZ71" s="18">
+        <v>6</v>
+      </c>
+      <c r="BA71" s="18">
+        <v>7</v>
+      </c>
+      <c r="BB71" s="18">
+        <v>8</v>
+      </c>
+      <c r="BC71" s="18">
+        <v>9</v>
+      </c>
+      <c r="BD71" s="18">
+        <v>10</v>
+      </c>
+      <c r="BE71" s="18">
+        <v>11</v>
+      </c>
+      <c r="BF71" s="18">
+        <v>12</v>
+      </c>
+      <c r="BG71" s="18">
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:59" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -5957,175 +5894,175 @@
         <v>65</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F72" s="18" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="G72" s="18" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="I72" s="26" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="J72" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="K72" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="L72" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="M72" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="N72" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="K72" s="26" t="s">
-        <v>282</v>
-      </c>
-      <c r="L72" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="M72" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="N72" s="26" t="s">
-        <v>297</v>
-      </c>
       <c r="O72" s="26" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="P72" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="Q72" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="R72" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="S72" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="Q72" s="26" t="s">
-        <v>311</v>
-      </c>
-      <c r="R72" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="S72" s="26" t="s">
+      <c r="T72" s="26" t="s">
+        <v>309</v>
+      </c>
+      <c r="U72" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="V72" s="26" t="s">
+        <v>318</v>
+      </c>
+      <c r="W72" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="T72" s="26" t="s">
+      <c r="X72" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="U72" s="26" t="s">
+      <c r="Y72" s="26" t="s">
         <v>334</v>
       </c>
-      <c r="V72" s="26" t="s">
-        <v>338</v>
-      </c>
-      <c r="W72" s="26" t="s">
-        <v>345</v>
-      </c>
-      <c r="X72" s="26" t="s">
-        <v>351</v>
-      </c>
-      <c r="Y72" s="26" t="s">
-        <v>356</v>
-      </c>
       <c r="Z72" s="26" t="s">
-        <v>361</v>
+        <v>339</v>
       </c>
       <c r="AA72" s="26" t="s">
+        <v>344</v>
+      </c>
+      <c r="AB72" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="AC72" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="AD72" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="AE72" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="AF72" s="26" t="s">
         <v>366</v>
       </c>
-      <c r="AB72" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="AC72" s="26" t="s">
-        <v>376</v>
-      </c>
-      <c r="AD72" s="26" t="s">
-        <v>379</v>
-      </c>
-      <c r="AE72" s="26" t="s">
-        <v>383</v>
-      </c>
-      <c r="AF72" s="26" t="s">
-        <v>389</v>
-      </c>
       <c r="AG72" s="26" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="AH72" s="26" t="s">
-        <v>402</v>
+        <v>377</v>
       </c>
       <c r="AI72" s="26" t="s">
-        <v>407</v>
+        <v>382</v>
       </c>
       <c r="AJ72" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="AK72" s="26" t="s">
+        <v>393</v>
+      </c>
+      <c r="AL72" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="AM72" s="26" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN72" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="AO72" s="26" t="s">
+        <v>409</v>
+      </c>
+      <c r="AP72" s="26" t="s">
         <v>412</v>
       </c>
-      <c r="AK72" s="26" t="s">
-        <v>418</v>
-      </c>
-      <c r="AL72" s="26" t="s">
-        <v>421</v>
-      </c>
-      <c r="AM72" s="26" t="s">
-        <v>421</v>
-      </c>
-      <c r="AN72" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="AO72" s="26" t="s">
-        <v>438</v>
-      </c>
-      <c r="AP72" s="26" t="s">
-        <v>442</v>
-      </c>
       <c r="AQ72" s="26" t="s">
-        <v>445</v>
+        <v>414</v>
       </c>
       <c r="AR72" s="26" t="s">
-        <v>449</v>
+        <v>417</v>
       </c>
       <c r="AS72" s="26" t="s">
-        <v>454</v>
+        <v>422</v>
       </c>
       <c r="AT72" s="26" t="s">
-        <v>458</v>
+        <v>426</v>
       </c>
       <c r="AU72" s="26" t="s">
-        <v>449</v>
+        <v>417</v>
       </c>
       <c r="AV72" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="AW72" s="26" t="s">
+        <v>435</v>
+      </c>
+      <c r="AX72" s="26" t="s">
+        <v>443</v>
+      </c>
+      <c r="AY72" s="26" t="s">
+        <v>448</v>
+      </c>
+      <c r="AZ72" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="BA72" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="BB72" s="26" t="s">
+        <v>457</v>
+      </c>
+      <c r="BC72" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="BD72" s="26" t="s">
+        <v>461</v>
+      </c>
+      <c r="BE72" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="BF72" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="BG72" s="26" t="s">
         <v>468</v>
-      </c>
-      <c r="AW72" s="26" t="s">
-        <v>468</v>
-      </c>
-      <c r="AX72" s="26" t="s">
-        <v>476</v>
-      </c>
-      <c r="AY72" s="26" t="s">
-        <v>481</v>
-      </c>
-      <c r="AZ72" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="BA72" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="BB72" s="26" t="s">
-        <v>490</v>
-      </c>
-      <c r="BC72" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="BD72" s="26" t="s">
-        <v>494</v>
-      </c>
-      <c r="BE72" s="26" t="s">
-        <v>288</v>
-      </c>
-      <c r="BF72" s="26" t="s">
-        <v>499</v>
-      </c>
-      <c r="BG72" s="26" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="73" spans="1:59" ht="29" x14ac:dyDescent="0.35">
@@ -6134,175 +6071,175 @@
         <v>66</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="E73" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="F73" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="G73" s="26" t="s">
+        <v>246</v>
+      </c>
+      <c r="H73" s="18" t="s">
         <v>251</v>
       </c>
-      <c r="F73" s="18" t="s">
+      <c r="I73" s="18" t="s">
         <v>256</v>
       </c>
-      <c r="G73" s="26" t="s">
+      <c r="J73" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="H73" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="I73" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="J73" s="26" t="s">
+      <c r="K73" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="L73" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="M73" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="N73" s="26" t="s">
         <v>279</v>
       </c>
-      <c r="K73" s="18" t="s">
-        <v>283</v>
-      </c>
-      <c r="L73" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="M73" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="N73" s="26" t="s">
-        <v>298</v>
-      </c>
       <c r="O73" s="26" t="s">
-        <v>301</v>
+        <v>282</v>
       </c>
       <c r="P73" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q73" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="R73" s="26" t="s">
+        <v>297</v>
+      </c>
+      <c r="S73" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="Q73" s="26" t="s">
-        <v>312</v>
-      </c>
-      <c r="R73" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="S73" s="26" t="s">
+      <c r="T73" s="26" t="s">
+        <v>310</v>
+      </c>
+      <c r="U73" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="V73" s="26" t="s">
+        <v>319</v>
+      </c>
+      <c r="W73" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="T73" s="26" t="s">
+      <c r="X73" s="26" t="s">
         <v>330</v>
       </c>
-      <c r="U73" s="26" t="s">
+      <c r="Y73" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="V73" s="26" t="s">
-        <v>339</v>
-      </c>
-      <c r="W73" s="26" t="s">
-        <v>346</v>
-      </c>
-      <c r="X73" s="26" t="s">
-        <v>352</v>
-      </c>
-      <c r="Y73" s="26" t="s">
-        <v>357</v>
-      </c>
       <c r="Z73" s="26" t="s">
-        <v>362</v>
+        <v>340</v>
       </c>
       <c r="AA73" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="AB73" s="26" t="s">
+        <v>349</v>
+      </c>
+      <c r="AC73" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="AD73" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="AE73" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="AF73" s="26" t="s">
         <v>367</v>
       </c>
-      <c r="AB73" s="26" t="s">
-        <v>371</v>
-      </c>
-      <c r="AC73" s="26" t="s">
-        <v>377</v>
-      </c>
-      <c r="AD73" s="26" t="s">
-        <v>380</v>
-      </c>
-      <c r="AE73" s="26" t="s">
-        <v>384</v>
-      </c>
-      <c r="AF73" s="26" t="s">
-        <v>390</v>
-      </c>
       <c r="AG73" s="26" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="AH73" s="26" t="s">
-        <v>403</v>
+        <v>378</v>
       </c>
       <c r="AI73" s="26" t="s">
-        <v>408</v>
+        <v>383</v>
       </c>
       <c r="AJ73" s="26" t="s">
-        <v>413</v>
+        <v>388</v>
       </c>
       <c r="AK73" s="26" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="AL73" s="26" t="s">
-        <v>422</v>
+        <v>397</v>
       </c>
       <c r="AM73" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="AN73" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="AO73" s="26" t="s">
+        <v>405</v>
+      </c>
+      <c r="AP73" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="AQ73" s="26" t="s">
+        <v>415</v>
+      </c>
+      <c r="AR73" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="AS73" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="AT73" s="26" t="s">
         <v>427</v>
       </c>
-      <c r="AN73" s="26" t="s">
-        <v>433</v>
-      </c>
-      <c r="AO73" s="26" t="s">
-        <v>433</v>
-      </c>
-      <c r="AP73" s="26" t="s">
-        <v>377</v>
-      </c>
-      <c r="AQ73" s="26" t="s">
-        <v>446</v>
-      </c>
-      <c r="AR73" s="26" t="s">
-        <v>450</v>
-      </c>
-      <c r="AS73" s="26" t="s">
-        <v>455</v>
-      </c>
-      <c r="AT73" s="26" t="s">
-        <v>459</v>
-      </c>
       <c r="AU73" s="26" t="s">
-        <v>463</v>
+        <v>430</v>
       </c>
       <c r="AV73" s="26" t="s">
+        <v>436</v>
+      </c>
+      <c r="AW73" s="26" t="s">
+        <v>441</v>
+      </c>
+      <c r="AX73" s="26" t="s">
+        <v>444</v>
+      </c>
+      <c r="AY73" s="26" t="s">
+        <v>449</v>
+      </c>
+      <c r="AZ73" s="26" t="s">
+        <v>451</v>
+      </c>
+      <c r="BA73" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="BB73" s="26" t="s">
+        <v>458</v>
+      </c>
+      <c r="BC73" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="BD73" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="BE73" s="26" t="s">
+        <v>454</v>
+      </c>
+      <c r="BF73" s="26" t="s">
+        <v>466</v>
+      </c>
+      <c r="BG73" s="26" t="s">
         <v>469</v>
-      </c>
-      <c r="AW73" s="26" t="s">
-        <v>474</v>
-      </c>
-      <c r="AX73" s="26" t="s">
-        <v>477</v>
-      </c>
-      <c r="AY73" s="26" t="s">
-        <v>482</v>
-      </c>
-      <c r="AZ73" s="26" t="s">
-        <v>484</v>
-      </c>
-      <c r="BA73" s="26" t="s">
-        <v>487</v>
-      </c>
-      <c r="BB73" s="26" t="s">
-        <v>491</v>
-      </c>
-      <c r="BC73" s="26" t="s">
-        <v>487</v>
-      </c>
-      <c r="BD73" s="26" t="s">
-        <v>495</v>
-      </c>
-      <c r="BE73" s="26" t="s">
-        <v>487</v>
-      </c>
-      <c r="BF73" s="26" t="s">
-        <v>500</v>
-      </c>
-      <c r="BG73" s="26" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="74" spans="1:59" ht="130.5" x14ac:dyDescent="0.35">
@@ -6311,175 +6248,175 @@
         <v>67</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="E74" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="F74" s="26" t="s">
+        <v>243</v>
+      </c>
+      <c r="G74" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="H74" s="26" t="s">
         <v>252</v>
       </c>
-      <c r="F74" s="26" t="s">
+      <c r="I74" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="G74" s="26" t="s">
+      <c r="J74" s="26" t="s">
         <v>262</v>
       </c>
-      <c r="H74" s="26" t="s">
-        <v>268</v>
-      </c>
-      <c r="I74" s="26" t="s">
-        <v>274</v>
-      </c>
-      <c r="J74" s="26" t="s">
+      <c r="K74" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="L74" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="M74" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="N74" s="26" t="s">
         <v>280</v>
       </c>
-      <c r="K74" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="L74" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="M74" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="N74" s="26" t="s">
-        <v>299</v>
-      </c>
       <c r="O74" s="26" t="s">
-        <v>302</v>
+        <v>283</v>
       </c>
       <c r="P74" s="26" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q74" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="R74" s="26" t="s">
+        <v>298</v>
+      </c>
+      <c r="S74" s="26" t="s">
         <v>306</v>
       </c>
-      <c r="Q74" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="R74" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="S74" s="26" t="s">
+      <c r="T74" s="26" t="s">
+        <v>311</v>
+      </c>
+      <c r="U74" s="26" t="s">
+        <v>316</v>
+      </c>
+      <c r="V74" s="26" t="s">
+        <v>320</v>
+      </c>
+      <c r="W74" s="26" t="s">
         <v>326</v>
       </c>
-      <c r="T74" s="26" t="s">
+      <c r="X74" s="26" t="s">
         <v>331</v>
       </c>
-      <c r="U74" s="26" t="s">
+      <c r="Y74" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="V74" s="26" t="s">
-        <v>340</v>
-      </c>
-      <c r="W74" s="26" t="s">
-        <v>347</v>
-      </c>
-      <c r="X74" s="26" t="s">
-        <v>353</v>
-      </c>
-      <c r="Y74" s="26" t="s">
-        <v>358</v>
-      </c>
       <c r="Z74" s="26" t="s">
-        <v>363</v>
+        <v>341</v>
       </c>
       <c r="AA74" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="AB74" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="AC74" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="AD74" s="26" t="s">
+        <v>359</v>
+      </c>
+      <c r="AE74" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="AF74" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="AB74" s="26" t="s">
-        <v>372</v>
-      </c>
-      <c r="AC74" s="26" t="s">
-        <v>378</v>
-      </c>
-      <c r="AD74" s="26" t="s">
-        <v>381</v>
-      </c>
-      <c r="AE74" s="26" t="s">
-        <v>385</v>
-      </c>
-      <c r="AF74" s="26" t="s">
+      <c r="AG74" s="26" t="s">
+        <v>373</v>
+      </c>
+      <c r="AH74" s="26" t="s">
+        <v>379</v>
+      </c>
+      <c r="AI74" s="26" t="s">
+        <v>384</v>
+      </c>
+      <c r="AJ74" s="26" t="s">
         <v>391</v>
       </c>
-      <c r="AG74" s="26" t="s">
-        <v>396</v>
-      </c>
-      <c r="AH74" s="26" t="s">
-        <v>404</v>
-      </c>
-      <c r="AI74" s="26" t="s">
-        <v>409</v>
-      </c>
-      <c r="AJ74" s="26" t="s">
+      <c r="AK74" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="AL74" s="26" t="s">
+        <v>398</v>
+      </c>
+      <c r="AM74" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="AN74" s="26" t="s">
+        <v>406</v>
+      </c>
+      <c r="AO74" s="26" t="s">
+        <v>410</v>
+      </c>
+      <c r="AP74" s="26" t="s">
+        <v>413</v>
+      </c>
+      <c r="AQ74" s="26" t="s">
         <v>416</v>
       </c>
-      <c r="AK74" s="26" t="s">
+      <c r="AR74" s="26" t="s">
         <v>419</v>
       </c>
-      <c r="AL74" s="26" t="s">
-        <v>423</v>
-      </c>
-      <c r="AM74" s="26" t="s">
+      <c r="AS74" s="26" t="s">
+        <v>424</v>
+      </c>
+      <c r="AT74" s="26" t="s">
         <v>428</v>
       </c>
-      <c r="AN74" s="26" t="s">
-        <v>434</v>
-      </c>
-      <c r="AO74" s="26" t="s">
-        <v>439</v>
-      </c>
-      <c r="AP74" s="26" t="s">
-        <v>443</v>
-      </c>
-      <c r="AQ74" s="26" t="s">
-        <v>447</v>
-      </c>
-      <c r="AR74" s="26" t="s">
-        <v>451</v>
-      </c>
-      <c r="AS74" s="26" t="s">
-        <v>456</v>
-      </c>
-      <c r="AT74" s="26" t="s">
+      <c r="AU74" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="AV74" s="26" t="s">
+        <v>437</v>
+      </c>
+      <c r="AW74" s="26" t="s">
+        <v>442</v>
+      </c>
+      <c r="AX74" s="26" t="s">
+        <v>445</v>
+      </c>
+      <c r="AY74" s="26" t="s">
+        <v>450</v>
+      </c>
+      <c r="AZ74" s="26" t="s">
+        <v>452</v>
+      </c>
+      <c r="BA74" s="26" t="s">
+        <v>455</v>
+      </c>
+      <c r="BB74" s="26" t="s">
+        <v>459</v>
+      </c>
+      <c r="BC74" s="26" t="s">
         <v>460</v>
       </c>
-      <c r="AU74" s="26" t="s">
+      <c r="BD74" s="26" t="s">
+        <v>463</v>
+      </c>
+      <c r="BE74" s="26" t="s">
         <v>464</v>
       </c>
-      <c r="AV74" s="26" t="s">
+      <c r="BF74" s="26" t="s">
+        <v>467</v>
+      </c>
+      <c r="BG74" s="26" t="s">
         <v>470</v>
-      </c>
-      <c r="AW74" s="26" t="s">
-        <v>475</v>
-      </c>
-      <c r="AX74" s="26" t="s">
-        <v>478</v>
-      </c>
-      <c r="AY74" s="26" t="s">
-        <v>483</v>
-      </c>
-      <c r="AZ74" s="26" t="s">
-        <v>485</v>
-      </c>
-      <c r="BA74" s="26" t="s">
-        <v>488</v>
-      </c>
-      <c r="BB74" s="26" t="s">
-        <v>492</v>
-      </c>
-      <c r="BC74" s="26" t="s">
-        <v>493</v>
-      </c>
-      <c r="BD74" s="26" t="s">
-        <v>496</v>
-      </c>
-      <c r="BE74" s="26" t="s">
-        <v>497</v>
-      </c>
-      <c r="BF74" s="26" t="s">
-        <v>501</v>
-      </c>
-      <c r="BG74" s="26" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="75" spans="1:59" x14ac:dyDescent="0.35">
@@ -6488,175 +6425,175 @@
         <v>68</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="E75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="G75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="I75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="J75" s="18" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="K75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="L75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="M75" s="18" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="N75" s="18" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="O75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="P75" s="18" t="s">
-        <v>307</v>
+        <v>288</v>
       </c>
       <c r="Q75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="R75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="S75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="T75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="U75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="V75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="W75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="X75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="Y75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="Z75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AA75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AB75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AC75" s="18" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="AD75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AE75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AF75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AG75" s="18" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="AH75" s="18" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="AI75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AJ75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AK75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AL75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AM75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AN75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AO75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AP75" s="18" t="s">
-        <v>295</v>
+        <v>276</v>
       </c>
       <c r="AQ75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AR75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AS75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AT75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AU75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AV75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AW75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AX75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="AY75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="AZ75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="BA75" s="18" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="BB75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="BC75" s="18" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="BD75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="BE75" s="18" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="BF75" s="18" t="s">
-        <v>319</v>
+        <v>299</v>
       </c>
       <c r="BG75" s="18" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:59" x14ac:dyDescent="0.35">
@@ -6665,175 +6602,175 @@
         <v>69</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="H76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="I76" s="18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="J76" s="18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="K76" s="18" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="L76" s="18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="M76" s="18" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="N76" s="18" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="O76" s="18" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="P76" s="18" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="Q76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="R76" s="18" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="S76" s="18" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="T76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="U76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="V76" s="18" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="W76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="X76" s="18" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="Y76" s="18" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="Z76" s="18" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
       <c r="AA76" s="18" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="AB76" s="18" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="AC76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="AD76" s="18" t="s">
-        <v>320</v>
+        <v>300</v>
       </c>
       <c r="AE76" s="18" t="s">
-        <v>386</v>
+        <v>363</v>
       </c>
       <c r="AF76" s="18" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="AG76" s="18" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="AH76" s="18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AI76" s="18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AJ76" s="18" t="s">
-        <v>414</v>
+        <v>389</v>
       </c>
       <c r="AK76" s="18" t="s">
-        <v>364</v>
+        <v>342</v>
       </c>
       <c r="AL76" s="18" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="AM76" s="18" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="AN76" s="18" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AO76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="AP76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="AQ76" s="18" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="AR76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="AS76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="AT76" s="18" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="AU76" s="18" t="s">
-        <v>465</v>
+        <v>432</v>
       </c>
       <c r="AV76" s="18" t="s">
-        <v>471</v>
+        <v>438</v>
       </c>
       <c r="AW76" s="18" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="AX76" s="18" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="AY76" s="18" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="AZ76" s="18" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="BA76" s="18" t="s">
-        <v>489</v>
+        <v>456</v>
       </c>
       <c r="BB76" s="18" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="BC76" s="18" t="s">
-        <v>489</v>
+        <v>456</v>
       </c>
       <c r="BD76" s="18" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="BE76" s="18" t="s">
-        <v>489</v>
+        <v>456</v>
       </c>
       <c r="BF76" s="18" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
       <c r="BG76" s="18" t="s">
-        <v>369</v>
+        <v>347</v>
       </c>
     </row>
     <row r="77" spans="1:59" x14ac:dyDescent="0.35">
@@ -7019,175 +6956,175 @@
         <v>71</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="D78" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="F78" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="G78" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="E78" s="18" t="s">
+      <c r="H78" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="F78" s="18" t="s">
+      <c r="I78" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="G78" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="H78" s="26" t="s">
-        <v>269</v>
-      </c>
-      <c r="I78" s="18" t="s">
-        <v>275</v>
-      </c>
       <c r="J78" s="18" t="s">
-        <v>275</v>
+        <v>258</v>
       </c>
       <c r="K78" s="18" t="s">
-        <v>286</v>
+        <v>268</v>
       </c>
       <c r="L78" s="18" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="M78" s="18" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="N78" s="18" t="s">
-        <v>291</v>
+        <v>272</v>
       </c>
       <c r="O78" s="18" t="s">
-        <v>303</v>
+        <v>284</v>
       </c>
       <c r="P78" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q78" s="18" t="s">
+        <v>294</v>
+      </c>
+      <c r="R78" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="S78" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="Q78" s="18" t="s">
-        <v>314</v>
-      </c>
-      <c r="R78" s="18" t="s">
-        <v>321</v>
-      </c>
-      <c r="S78" s="26" t="s">
-        <v>328</v>
-      </c>
       <c r="T78" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="U78" s="26" t="s">
+        <v>317</v>
+      </c>
+      <c r="V78" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="W78" s="18" t="s">
+        <v>327</v>
+      </c>
+      <c r="X78" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="U78" s="26" t="s">
+      <c r="Y78" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="V78" s="18" t="s">
-        <v>342</v>
-      </c>
-      <c r="W78" s="18" t="s">
-        <v>348</v>
-      </c>
-      <c r="X78" s="18" t="s">
-        <v>354</v>
-      </c>
-      <c r="Y78" s="18" t="s">
-        <v>359</v>
-      </c>
       <c r="Z78" s="18" t="s">
-        <v>359</v>
+        <v>337</v>
       </c>
       <c r="AA78" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="AB78" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="AC78" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="AD78" s="18" t="s">
+        <v>351</v>
+      </c>
+      <c r="AE78" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="AF78" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="AG78" s="18" t="s">
         <v>375</v>
       </c>
-      <c r="AB78" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="AC78" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="AD78" s="18" t="s">
-        <v>373</v>
-      </c>
-      <c r="AE78" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="AF78" s="26" t="s">
-        <v>392</v>
-      </c>
-      <c r="AG78" s="18" t="s">
-        <v>398</v>
-      </c>
       <c r="AH78" s="18" t="s">
-        <v>405</v>
+        <v>380</v>
       </c>
       <c r="AI78" s="18" t="s">
-        <v>410</v>
+        <v>385</v>
       </c>
       <c r="AJ78" s="26" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="AK78" s="26" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="AL78" s="26" t="s">
-        <v>424</v>
+        <v>399</v>
       </c>
       <c r="AM78" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="AN78" s="26" t="s">
+        <v>407</v>
+      </c>
+      <c r="AO78" s="26" t="s">
+        <v>407</v>
+      </c>
+      <c r="AP78" s="26" t="s">
+        <v>407</v>
+      </c>
+      <c r="AQ78" s="26" t="s">
+        <v>407</v>
+      </c>
+      <c r="AR78" s="26" t="s">
+        <v>420</v>
+      </c>
+      <c r="AS78" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="AT78" s="26" t="s">
         <v>429</v>
       </c>
-      <c r="AN78" s="26" t="s">
-        <v>435</v>
-      </c>
-      <c r="AO78" s="26" t="s">
-        <v>435</v>
-      </c>
-      <c r="AP78" s="26" t="s">
-        <v>435</v>
-      </c>
-      <c r="AQ78" s="26" t="s">
-        <v>435</v>
-      </c>
-      <c r="AR78" s="26" t="s">
-        <v>452</v>
-      </c>
-      <c r="AS78" s="26" t="s">
-        <v>457</v>
-      </c>
-      <c r="AT78" s="26" t="s">
-        <v>461</v>
-      </c>
       <c r="AU78" s="26" t="s">
-        <v>466</v>
+        <v>433</v>
       </c>
       <c r="AV78" s="26" t="s">
-        <v>472</v>
+        <v>439</v>
       </c>
       <c r="AW78" s="26" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="AX78" s="26" t="s">
-        <v>479</v>
+        <v>446</v>
       </c>
       <c r="AY78" s="26" t="s">
-        <v>479</v>
+        <v>446</v>
       </c>
       <c r="AZ78" s="26" t="s">
-        <v>486</v>
+        <v>453</v>
       </c>
       <c r="BA78" s="26" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="BB78" s="26" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="BC78" s="26" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="BD78" s="26" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="BE78" s="26" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="BF78" s="26" t="s">
-        <v>415</v>
+        <v>390</v>
       </c>
       <c r="BG78" s="26" t="s">
-        <v>506</v>
+        <v>471</v>
       </c>
     </row>
     <row r="79" spans="1:59" ht="43.5" x14ac:dyDescent="0.35">
@@ -7196,142 +7133,142 @@
         <v>77</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="D79" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="E79" s="26" t="s">
+        <v>241</v>
+      </c>
+      <c r="F79" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="G79" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="E79" s="26" t="s">
+      <c r="H79" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="F79" s="18" t="s">
+      <c r="I79" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="G79" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="H79" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="I79" s="18" t="s">
-        <v>276</v>
-      </c>
       <c r="J79" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="K79" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="L79" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="M79" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="N79" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="K79" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="L79" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="M79" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="N79" s="26" t="s">
-        <v>300</v>
-      </c>
       <c r="O79" s="18" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="P79" s="26" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="Q79" s="26" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="R79" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="S79" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="T79" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="U79" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="V79" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="S79" s="26" t="s">
-        <v>323</v>
-      </c>
-      <c r="T79" s="26" t="s">
+      <c r="W79" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="X79" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="U79" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="V79" s="26" t="s">
+      <c r="Y79" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="Z79" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="W79" s="26" t="s">
-        <v>349</v>
-      </c>
-      <c r="X79" s="26" t="s">
-        <v>355</v>
-      </c>
-      <c r="Y79" s="26" t="s">
-        <v>360</v>
-      </c>
-      <c r="Z79" s="26" t="s">
-        <v>365</v>
-      </c>
       <c r="AA79" s="26" t="s">
-        <v>370</v>
+        <v>348</v>
       </c>
       <c r="AB79" s="26" t="s">
-        <v>374</v>
+        <v>352</v>
       </c>
       <c r="AC79" s="26"/>
       <c r="AD79" s="26"/>
       <c r="AE79" s="26" t="s">
-        <v>388</v>
+        <v>365</v>
       </c>
       <c r="AF79" s="26" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
       <c r="AG79" s="26" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="AH79" s="26" t="s">
-        <v>406</v>
+        <v>381</v>
       </c>
       <c r="AI79" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="AJ79" s="26" t="s">
+        <v>392</v>
+      </c>
+      <c r="AK79" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="AL79" s="26" t="s">
+        <v>400</v>
+      </c>
+      <c r="AM79" s="26" t="s">
+        <v>404</v>
+      </c>
+      <c r="AN79" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="AO79" s="26" t="s">
         <v>411</v>
-      </c>
-      <c r="AJ79" s="26" t="s">
-        <v>417</v>
-      </c>
-      <c r="AK79" s="26" t="s">
-        <v>420</v>
-      </c>
-      <c r="AL79" s="26" t="s">
-        <v>425</v>
-      </c>
-      <c r="AM79" s="26" t="s">
-        <v>430</v>
-      </c>
-      <c r="AN79" s="26" t="s">
-        <v>436</v>
-      </c>
-      <c r="AO79" s="26" t="s">
-        <v>440</v>
       </c>
       <c r="AP79" s="26"/>
       <c r="AQ79" s="26"/>
       <c r="AR79" s="26" t="s">
-        <v>453</v>
+        <v>421</v>
       </c>
       <c r="AS79" s="26" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
       <c r="AT79" s="26" t="s">
-        <v>457</v>
+        <v>425</v>
       </c>
       <c r="AU79" s="26" t="s">
-        <v>467</v>
+        <v>434</v>
       </c>
       <c r="AV79" s="26" t="s">
-        <v>473</v>
+        <v>440</v>
       </c>
       <c r="AW79" s="26"/>
       <c r="AX79" s="26" t="s">
-        <v>480</v>
+        <v>447</v>
       </c>
       <c r="AY79" s="26"/>
       <c r="AZ79" s="26" t="s">
-        <v>480</v>
+        <v>447</v>
       </c>
       <c r="BA79" s="26"/>
       <c r="BB79" s="26"/>
@@ -7340,7 +7277,7 @@
       <c r="BE79" s="26"/>
       <c r="BF79" s="26"/>
       <c r="BG79" s="26" t="s">
-        <v>507</v>
+        <v>472</v>
       </c>
     </row>
     <row r="80" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7432,112 +7369,112 @@
         <v>74</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>508</v>
+        <v>473</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>511</v>
+        <v>476</v>
       </c>
       <c r="E82" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="F82" s="18" t="s">
+        <v>482</v>
+      </c>
+      <c r="G82" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="H82" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="I82" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="J82" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="K82" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="L82" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="M82" s="18" t="s">
+        <v>503</v>
+      </c>
+      <c r="N82" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="O82" s="18" t="s">
+        <v>507</v>
+      </c>
+      <c r="P82" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q82" s="18" t="s">
+        <v>512</v>
+      </c>
+      <c r="R82" s="18" t="s">
         <v>514</v>
       </c>
-      <c r="F82" s="18" t="s">
-        <v>517</v>
-      </c>
-      <c r="G82" s="18" t="s">
+      <c r="S82" s="18" t="s">
+        <v>518</v>
+      </c>
+      <c r="T82" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="H82" s="18" t="s">
-        <v>523</v>
-      </c>
-      <c r="I82" s="18" t="s">
-        <v>526</v>
-      </c>
-      <c r="J82" s="18" t="s">
-        <v>315</v>
-      </c>
-      <c r="K82" s="18" t="s">
-        <v>531</v>
-      </c>
-      <c r="L82" s="18" t="s">
-        <v>534</v>
-      </c>
-      <c r="M82" s="18" t="s">
+      <c r="U82" s="18" t="s">
+        <v>524</v>
+      </c>
+      <c r="V82" s="18" t="s">
+        <v>527</v>
+      </c>
+      <c r="W82" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="X82" s="18" t="s">
+        <v>532</v>
+      </c>
+      <c r="Y82" s="18" t="s">
+        <v>535</v>
+      </c>
+      <c r="Z82" s="18" t="s">
         <v>538</v>
       </c>
-      <c r="N82" s="18" t="s">
-        <v>540</v>
-      </c>
-      <c r="O82" s="18" t="s">
-        <v>542</v>
-      </c>
-      <c r="P82" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="Q82" s="18" t="s">
+      <c r="AA82" s="18" t="s">
+        <v>541</v>
+      </c>
+      <c r="AB82" s="18" t="s">
+        <v>544</v>
+      </c>
+      <c r="AC82" s="18" t="s">
         <v>547</v>
       </c>
-      <c r="R82" s="18" t="s">
-        <v>549</v>
-      </c>
-      <c r="S82" s="18" t="s">
-        <v>553</v>
-      </c>
-      <c r="T82" s="18" t="s">
+      <c r="AD82" s="18" t="s">
+        <v>550</v>
+      </c>
+      <c r="AE82" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="AF82" s="18" t="s">
         <v>555</v>
       </c>
-      <c r="U82" s="18" t="s">
+      <c r="AG82" s="18" t="s">
+        <v>557</v>
+      </c>
+      <c r="AH82" s="18" t="s">
         <v>559</v>
       </c>
-      <c r="V82" s="18" t="s">
+      <c r="AI82" s="18" t="s">
         <v>562</v>
       </c>
-      <c r="W82" s="18" t="s">
+      <c r="AJ82" s="18" t="s">
         <v>565</v>
       </c>
-      <c r="X82" s="18" t="s">
-        <v>567</v>
-      </c>
-      <c r="Y82" s="18" t="s">
-        <v>570</v>
-      </c>
-      <c r="Z82" s="18" t="s">
-        <v>573</v>
-      </c>
-      <c r="AA82" s="18" t="s">
-        <v>576</v>
-      </c>
-      <c r="AB82" s="18" t="s">
-        <v>579</v>
-      </c>
-      <c r="AC82" s="18" t="s">
-        <v>582</v>
-      </c>
-      <c r="AD82" s="18" t="s">
-        <v>585</v>
-      </c>
-      <c r="AE82" s="18" t="s">
-        <v>587</v>
-      </c>
-      <c r="AF82" s="18" t="s">
-        <v>590</v>
-      </c>
-      <c r="AG82" s="18" t="s">
-        <v>592</v>
-      </c>
-      <c r="AH82" s="18" t="s">
-        <v>594</v>
-      </c>
-      <c r="AI82" s="18" t="s">
-        <v>597</v>
-      </c>
-      <c r="AJ82" s="18" t="s">
-        <v>600</v>
-      </c>
       <c r="AK82" s="18" t="s">
-        <v>603</v>
+        <v>568</v>
       </c>
       <c r="AL82" s="18" t="s">
-        <v>606</v>
+        <v>571</v>
       </c>
     </row>
     <row r="83" spans="1:38" x14ac:dyDescent="0.35">
@@ -7546,112 +7483,112 @@
         <v>75</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>509</v>
+        <v>474</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>512</v>
+        <v>477</v>
       </c>
       <c r="E83" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="F83" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="G83" s="18" t="s">
+        <v>486</v>
+      </c>
+      <c r="H83" s="18" t="s">
+        <v>489</v>
+      </c>
+      <c r="I83" s="18" t="s">
+        <v>492</v>
+      </c>
+      <c r="J83" s="18" t="s">
+        <v>494</v>
+      </c>
+      <c r="K83" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="L83" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="M83" s="18" t="s">
+        <v>502</v>
+      </c>
+      <c r="N83" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="O83" s="18" t="s">
+        <v>508</v>
+      </c>
+      <c r="P83" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="Q83" s="18" t="s">
+        <v>516</v>
+      </c>
+      <c r="R83" s="18" t="s">
         <v>515</v>
       </c>
-      <c r="F83" s="18" t="s">
-        <v>518</v>
-      </c>
-      <c r="G83" s="18" t="s">
+      <c r="S83" s="18" t="s">
         <v>521</v>
       </c>
-      <c r="H83" s="18" t="s">
-        <v>524</v>
-      </c>
-      <c r="I83" s="18" t="s">
-        <v>527</v>
-      </c>
-      <c r="J83" s="18" t="s">
-        <v>529</v>
-      </c>
-      <c r="K83" s="18" t="s">
-        <v>532</v>
-      </c>
-      <c r="L83" s="18" t="s">
-        <v>535</v>
-      </c>
-      <c r="M83" s="18" t="s">
-        <v>537</v>
-      </c>
-      <c r="N83" s="18" t="s">
-        <v>535</v>
-      </c>
-      <c r="O83" s="18" t="s">
-        <v>543</v>
-      </c>
-      <c r="P83" s="18" t="s">
+      <c r="T83" s="18" t="s">
+        <v>522</v>
+      </c>
+      <c r="U83" s="18" t="s">
+        <v>525</v>
+      </c>
+      <c r="V83" s="18" t="s">
+        <v>528</v>
+      </c>
+      <c r="W83" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="X83" s="18" t="s">
+        <v>533</v>
+      </c>
+      <c r="Y83" s="18" t="s">
+        <v>536</v>
+      </c>
+      <c r="Z83" s="18" t="s">
+        <v>539</v>
+      </c>
+      <c r="AA83" s="18" t="s">
+        <v>542</v>
+      </c>
+      <c r="AB83" s="18" t="s">
         <v>545</v>
       </c>
-      <c r="Q83" s="18" t="s">
+      <c r="AC83" s="18" t="s">
+        <v>548</v>
+      </c>
+      <c r="AD83" s="18" t="s">
         <v>551</v>
       </c>
-      <c r="R83" s="18" t="s">
-        <v>550</v>
-      </c>
-      <c r="S83" s="18" t="s">
+      <c r="AE83" s="18" t="s">
+        <v>553</v>
+      </c>
+      <c r="AF83" s="18" t="s">
         <v>556</v>
       </c>
-      <c r="T83" s="18" t="s">
-        <v>557</v>
-      </c>
-      <c r="U83" s="18" t="s">
+      <c r="AG83" s="18" t="s">
+        <v>558</v>
+      </c>
+      <c r="AH83" s="18" t="s">
         <v>560</v>
       </c>
-      <c r="V83" s="18" t="s">
+      <c r="AI83" s="18" t="s">
         <v>563</v>
       </c>
-      <c r="W83" s="18" t="s">
-        <v>356</v>
-      </c>
-      <c r="X83" s="18" t="s">
-        <v>568</v>
-      </c>
-      <c r="Y83" s="18" t="s">
-        <v>571</v>
-      </c>
-      <c r="Z83" s="18" t="s">
-        <v>574</v>
-      </c>
-      <c r="AA83" s="18" t="s">
-        <v>577</v>
-      </c>
-      <c r="AB83" s="18" t="s">
-        <v>580</v>
-      </c>
-      <c r="AC83" s="18" t="s">
-        <v>583</v>
-      </c>
-      <c r="AD83" s="18" t="s">
-        <v>586</v>
-      </c>
-      <c r="AE83" s="18" t="s">
-        <v>588</v>
-      </c>
-      <c r="AF83" s="18" t="s">
-        <v>591</v>
-      </c>
-      <c r="AG83" s="18" t="s">
-        <v>593</v>
-      </c>
-      <c r="AH83" s="18" t="s">
-        <v>595</v>
-      </c>
-      <c r="AI83" s="18" t="s">
-        <v>598</v>
-      </c>
       <c r="AJ83" s="18" t="s">
-        <v>601</v>
+        <v>566</v>
       </c>
       <c r="AK83" s="18" t="s">
-        <v>604</v>
+        <v>569</v>
       </c>
       <c r="AL83" s="18" t="s">
-        <v>607</v>
+        <v>572</v>
       </c>
     </row>
     <row r="84" spans="1:38" ht="72.5" x14ac:dyDescent="0.35">
@@ -7660,110 +7597,110 @@
         <v>76</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>510</v>
+        <v>475</v>
       </c>
       <c r="D84" s="18" t="s">
+        <v>478</v>
+      </c>
+      <c r="E84" s="26" t="s">
+        <v>481</v>
+      </c>
+      <c r="F84" s="26" t="s">
+        <v>484</v>
+      </c>
+      <c r="G84" s="26" t="s">
+        <v>487</v>
+      </c>
+      <c r="H84" s="26" t="s">
+        <v>490</v>
+      </c>
+      <c r="I84" s="26" t="s">
+        <v>493</v>
+      </c>
+      <c r="J84" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="K84" s="26" t="s">
+        <v>498</v>
+      </c>
+      <c r="L84" s="26" t="s">
+        <v>501</v>
+      </c>
+      <c r="M84" s="26" t="s">
+        <v>504</v>
+      </c>
+      <c r="N84" s="26" t="s">
+        <v>506</v>
+      </c>
+      <c r="O84" s="26" t="s">
+        <v>509</v>
+      </c>
+      <c r="P84" s="26" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q84" s="26" t="s">
         <v>513</v>
       </c>
-      <c r="E84" s="26" t="s">
-        <v>516</v>
-      </c>
-      <c r="F84" s="26" t="s">
+      <c r="R84" s="26" t="s">
+        <v>517</v>
+      </c>
+      <c r="S84" s="26" t="s">
         <v>519</v>
       </c>
-      <c r="G84" s="26" t="s">
-        <v>522</v>
-      </c>
-      <c r="H84" s="26" t="s">
-        <v>525</v>
-      </c>
-      <c r="I84" s="26" t="s">
-        <v>528</v>
-      </c>
-      <c r="J84" s="26" t="s">
-        <v>530</v>
-      </c>
-      <c r="K84" s="26" t="s">
-        <v>533</v>
-      </c>
-      <c r="L84" s="26" t="s">
-        <v>536</v>
-      </c>
-      <c r="M84" s="26" t="s">
-        <v>539</v>
-      </c>
-      <c r="N84" s="26" t="s">
-        <v>541</v>
-      </c>
-      <c r="O84" s="26" t="s">
-        <v>544</v>
-      </c>
-      <c r="P84" s="26" t="s">
+      <c r="T84" s="26" t="s">
+        <v>523</v>
+      </c>
+      <c r="U84" s="26" t="s">
+        <v>526</v>
+      </c>
+      <c r="V84" s="26" t="s">
+        <v>529</v>
+      </c>
+      <c r="W84" s="26" t="s">
+        <v>531</v>
+      </c>
+      <c r="X84" s="26" t="s">
+        <v>534</v>
+      </c>
+      <c r="Y84" s="26" t="s">
+        <v>537</v>
+      </c>
+      <c r="Z84" s="26" t="s">
+        <v>540</v>
+      </c>
+      <c r="AA84" s="26" t="s">
+        <v>543</v>
+      </c>
+      <c r="AB84" s="26" t="s">
         <v>546</v>
       </c>
-      <c r="Q84" s="26" t="s">
-        <v>548</v>
-      </c>
-      <c r="R84" s="26" t="s">
-        <v>552</v>
-      </c>
-      <c r="S84" s="26" t="s">
-        <v>554</v>
-      </c>
-      <c r="T84" s="26" t="s">
-        <v>558</v>
-      </c>
-      <c r="U84" s="26" t="s">
-        <v>561</v>
-      </c>
-      <c r="V84" s="26" t="s">
-        <v>564</v>
-      </c>
-      <c r="W84" s="26" t="s">
-        <v>566</v>
-      </c>
-      <c r="X84" s="26" t="s">
-        <v>569</v>
-      </c>
-      <c r="Y84" s="26" t="s">
-        <v>572</v>
-      </c>
-      <c r="Z84" s="26" t="s">
-        <v>575</v>
-      </c>
-      <c r="AA84" s="26" t="s">
-        <v>578</v>
-      </c>
-      <c r="AB84" s="26" t="s">
-        <v>581</v>
-      </c>
       <c r="AC84" s="26" t="s">
-        <v>584</v>
+        <v>549</v>
       </c>
       <c r="AD84" s="26"/>
       <c r="AE84" s="26" t="s">
-        <v>589</v>
+        <v>554</v>
       </c>
       <c r="AF84" s="26" t="s">
-        <v>613</v>
+        <v>578</v>
       </c>
       <c r="AG84" s="26" t="s">
-        <v>614</v>
+        <v>579</v>
       </c>
       <c r="AH84" s="26" t="s">
-        <v>596</v>
+        <v>561</v>
       </c>
       <c r="AI84" s="26" t="s">
-        <v>599</v>
+        <v>564</v>
       </c>
       <c r="AJ84" s="26" t="s">
-        <v>602</v>
+        <v>567</v>
       </c>
       <c r="AK84" s="26" t="s">
-        <v>605</v>
+        <v>570</v>
       </c>
       <c r="AL84" s="26" t="s">
-        <v>608</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct steps - scenarios section
</commit_message>
<xml_diff>
--- a/excel-use-cases/MAESHA/IEC62559-2_TEMPLATE_FrequencyControlUC.xlsx
+++ b/excel-use-cases/MAESHA/IEC62559-2_TEMPLATE_FrequencyControlUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MAESHA\08_BRIDGE\Data Management WG\UC repository\MAESHA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAF5768-059A-4AA1-831F-5AE119D9538A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3AC089-06B8-4A17-A9FC-0BE4304463C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1363,7 +1363,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="563">
   <si>
     <t>1 Description of the use case</t>
   </si>
@@ -2064,9 +2064,6 @@
     <t>IE-01-01 (frequency bandwigth and emergency thresholds)</t>
   </si>
   <si>
-    <t>R-01-01 (guidelines for operation defined by regulator)</t>
-  </si>
-  <si>
     <t>Collect data of the power system</t>
   </si>
   <si>
@@ -2081,9 +2078,6 @@
 IE-01-04 (fault statistics)</t>
   </si>
   <si>
-    <t>R-01-02 (historic data about electricity system, load and frequency)</t>
-  </si>
-  <si>
     <t>Mid-term &amp; long-term forecasts</t>
   </si>
   <si>
@@ -2093,9 +2087,6 @@
     <t>IE-01-05 (mid-term &amp; long-term forecasts)</t>
   </si>
   <si>
-    <t>R-01-03 (List of planned new DER installations)</t>
-  </si>
-  <si>
     <t>Define design scenarios</t>
   </si>
   <si>
@@ -2105,9 +2096,6 @@
     <t>IE-01-06 (design scenarios)</t>
   </si>
   <si>
-    <t>IE-01, IE-02, IE-03, IE-04, IE-05 received</t>
-  </si>
-  <si>
     <t>Calculate the required amount of flexibility- balancing reserve needed on the island - FRR</t>
   </si>
   <si>
@@ -2117,9 +2105,6 @@
     <t>IE-01-07 (required amount of balancing reserve)</t>
   </si>
   <si>
-    <t>IE-01, IE-02, IE-03, IE-04, IE-05, IE-06 received</t>
-  </si>
-  <si>
     <t>St5 finished</t>
   </si>
   <si>
@@ -2132,9 +2117,6 @@
     <t>IE-01-08 (definition of balancing products and requirements)</t>
   </si>
   <si>
-    <t>IE-01-07 received</t>
-  </si>
-  <si>
     <t>Periodically (interval of 1s of faster)</t>
   </si>
   <si>
@@ -2147,9 +2129,6 @@
     <t>IE-02-01 (Network frequency)</t>
   </si>
   <si>
-    <t>R-02-01 (frequency meter on-site)</t>
-  </si>
-  <si>
     <t>New frequency measurement available</t>
   </si>
   <si>
@@ -2159,9 +2138,6 @@
     <t>The measured frequency must be sent to the local controller capable of receiving freq. measurements in real-time</t>
   </si>
   <si>
-    <t>R-02-02 (on-site PLC)</t>
-  </si>
-  <si>
     <t>When freq. measurements arrive to the local controller</t>
   </si>
   <si>
@@ -2189,9 +2165,6 @@
     <t>IE-03-01 (grid frequency)</t>
   </si>
   <si>
-    <t>R-03-01 (central frequency meter)</t>
-  </si>
-  <si>
     <t>Receive frequency measurement</t>
   </si>
   <si>
@@ -2201,9 +2174,6 @@
     <t>REPORT</t>
   </si>
   <si>
-    <t>R-03-02 (AGC)</t>
-  </si>
-  <si>
     <t>Frequency measurement received by AGC</t>
   </si>
   <si>
@@ -2213,9 +2183,6 @@
     <t>The frequency measurements need to be persisted and available in real time and for later analysis. The SCADA (where AGC is embedded) saved the measurements in a database.</t>
   </si>
   <si>
-    <t>R-03-03 (data storage)</t>
-  </si>
-  <si>
     <t>Calculate the frequency deviation</t>
   </si>
   <si>
@@ -2240,9 +2207,6 @@
     <t>IE-03-03 (updated FRR setpoint)</t>
   </si>
   <si>
-    <t>R-03-04 (P-f- control algorithm)</t>
-  </si>
-  <si>
     <t xml:space="preserve">After definition of technical require-ments </t>
   </si>
   <si>
@@ -2279,9 +2243,6 @@
     <t>IE-04-01</t>
   </si>
   <si>
-    <t>IE-04-01 available</t>
-  </si>
-  <si>
     <t>After reception of tender announcement</t>
   </si>
   <si>
@@ -2309,9 +2270,6 @@
     <t>IE-04-04 (confirmation of prequalification)</t>
   </si>
   <si>
-    <t>IE-04-02 or IE-04-03 available</t>
-  </si>
-  <si>
     <t>Periodically (yearly, monthly, weekly, or daily)</t>
   </si>
   <si>
@@ -2339,9 +2297,6 @@
     <t>IE-04-06 (balancing service bid document)</t>
   </si>
   <si>
-    <t>IE-04-05, R-04-01 (prequalified flexibility providers)</t>
-  </si>
-  <si>
     <t>SO received bid for balancing service provision</t>
   </si>
   <si>
@@ -2354,9 +2309,6 @@
     <t>IE-04-07 (balancing service bid acceptance)</t>
   </si>
   <si>
-    <t>IE-04-06 received</t>
-  </si>
-  <si>
     <t>Reception of FCR bid acceptance</t>
   </si>
   <si>
@@ -2369,9 +2321,6 @@
     <t>IE-05-01 (FCR provision enabled)</t>
   </si>
   <si>
-    <t>IE-04-07 (accepted FCR bid)</t>
-  </si>
-  <si>
     <t>FCR provision enabled</t>
   </si>
   <si>
@@ -2384,10 +2333,6 @@
     <t>IE-05-02 (FCR setpoint)</t>
   </si>
   <si>
-    <t>IE-02-02 (frequency deviation)
-R-05-01 (P(Df) characteristics implemented)</t>
-  </si>
-  <si>
     <t>FCR setpoint calculated (continuously, e.g., 1s interval)</t>
   </si>
   <si>
@@ -2400,9 +2345,6 @@
     <t>DER</t>
   </si>
   <si>
-    <t>R-05-02 (DER operative)</t>
-  </si>
-  <si>
     <t>Continuously (e.g., 1s interval)</t>
   </si>
   <si>
@@ -2415,10 +2357,6 @@
     <t>PLC (DER)</t>
   </si>
   <si>
-    <t>R-05-03 (communication. channel between PLC and FMTP)
-R-05-05 (active power meter (on-site))</t>
-  </si>
-  <si>
     <t>Validate FCR provision</t>
   </si>
   <si>
@@ -2428,9 +2366,6 @@
     <t>IE-05-04 (FCR validation report)</t>
   </si>
   <si>
-    <t>R-05-04 (algorithm to validate FCR performance)</t>
-  </si>
-  <si>
     <t xml:space="preserve">IE-05-03 (FCR monitoring data) </t>
   </si>
   <si>
@@ -2465,9 +2400,6 @@
   </si>
   <si>
     <t>IE-06-01 (FRR provision enabled)</t>
-  </si>
-  <si>
-    <t>IE-04-07 (accepted FRR bid)</t>
   </si>
   <si>
     <t>New FRR setpoint available</t>
@@ -2483,9 +2415,6 @@
 IE-06-03 (setpoint for DER)</t>
   </si>
   <si>
-    <t>R-06-01 (dispatching algorithm)</t>
-  </si>
-  <si>
     <t>Central assets’ FRR setpoint updated</t>
   </si>
   <si>
@@ -2501,9 +2430,6 @@
     <t>IE-06-02 (setpoints for central balancing assets)</t>
   </si>
   <si>
-    <t>R-06-02 (central balancing asset available)</t>
-  </si>
-  <si>
     <t>Decentral assets’ FRR setpoint updated</t>
   </si>
   <si>
@@ -2516,10 +2442,6 @@
     <t>IE-06-03 (setpoint for DER)</t>
   </si>
   <si>
-    <t>R-06-03 (FMTP available)
-R-06-07 (comm. channel between AGC and FMTP)</t>
-  </si>
-  <si>
     <t>FMTP received a new FRR setpoint</t>
   </si>
   <si>
@@ -2532,10 +2454,6 @@
     <t>IE-06-04 (activation requests)</t>
   </si>
   <si>
-    <t>R-06-03 (FMTP available)
-R-06-06 (communication channel between FMTP and intermediate platforms or large DER)</t>
-  </si>
-  <si>
     <t>Intermediate platform receives activation request</t>
   </si>
   <si>
@@ -2551,19 +2469,12 @@
     <t>The intermediate platform disaggregates the received activation request and forwards the setpoints to the connected DER, which previously indicated availability.</t>
   </si>
   <si>
-    <t>R-06-04 (DER available)
-R-06-05 (communication channel between DER and intermediate platform)</t>
-  </si>
-  <si>
     <t>DER received the activation request</t>
   </si>
   <si>
     <t>The DER changes its generation or consumption according to the received setpoint within the required FAT (details see scenario 8).</t>
   </si>
   <si>
-    <t>R-06-04 (DER available)</t>
-  </si>
-  <si>
     <t>Continuously (e.g., in 2s interval)</t>
   </si>
   <si>
@@ -2574,10 +2485,6 @@
   </si>
   <si>
     <t>IE-06-06 (individual FRR moni-toring data)</t>
-  </si>
-  <si>
-    <t>R-06-05 (communication channel between DER and intermediate platform)
-R-05-05 (active power meter, on-site)</t>
   </si>
   <si>
     <t>Send monitoring data to AGC</t>
@@ -2590,9 +2497,6 @@
     <t>IE-06-07 (aggregated FRR monitoring data)</t>
   </si>
   <si>
-    <t>R-06-06 (communication channel between FMTP and intermediate platforms or large DER)</t>
-  </si>
-  <si>
     <t>Validate FRR provision</t>
   </si>
   <si>
@@ -2602,16 +2506,10 @@
     <t>IE-06-08 (FRR validation report)</t>
   </si>
   <si>
-    <t>R-06-08 (algorithm to validate FRR performance)</t>
-  </si>
-  <si>
     <t>Yearly</t>
   </si>
   <si>
     <t>In case of doubts, the SO compares FRR monitoring data with (public) meter readings.</t>
-  </si>
-  <si>
-    <t>R-06-09 (meter data)</t>
   </si>
   <si>
     <t>FRR malperformance detected</t>
@@ -2642,10 +2540,6 @@
 IE-06-07 (monitoring data)</t>
   </si>
   <si>
-    <t>IE-06-08 (FRR validation report)
-IE-05-04 (FCR validation report)</t>
-  </si>
-  <si>
     <t>After completing previous step</t>
   </si>
   <si>
@@ -2682,9 +2576,6 @@
     <t>IE-08-01 (forecast of flexible capacity and costs)</t>
   </si>
   <si>
-    <t>R-08-01 (Operational forecast of DER)</t>
-  </si>
-  <si>
     <t>Previous step finalized</t>
   </si>
   <si>
@@ -2698,10 +2589,6 @@
   </si>
   <si>
     <t>IE-08-02 (flexibility merit order)</t>
-  </si>
-  <si>
-    <t>IE-08-01
-R-06-05 (communication channel between DER and intermediate platform)</t>
   </si>
   <si>
     <t>Participation in balancing service tender</t>
@@ -2723,9 +2610,6 @@
     <t>IE-08-02 (Flexibility reservation request)</t>
   </si>
   <si>
-    <t>R-06-05 (communication channel between DER and intermediate platform)</t>
-  </si>
-  <si>
     <t>Flexibility reservation request received</t>
   </si>
   <si>
@@ -2796,9 +2680,6 @@
   </si>
   <si>
     <t>IE-06-06 (individual FRR monitoring data)</t>
-  </si>
-  <si>
-    <t>R-05-05 (active power meter (on-site))</t>
   </si>
   <si>
     <t>IE-01-01</t>
@@ -3470,15 +3351,6 @@
     <t>9b</t>
   </si>
   <si>
-    <t>Detection of the frequency issues - Frequency Containment Reservce (FCR)</t>
-  </si>
-  <si>
-    <t>Detection of the frequency issues - Frequency Restoration Reserve (FRR)</t>
-  </si>
-  <si>
-    <t>Flexibility activation through the Flexibility Management and Trading Platform - FRR</t>
-  </si>
-  <si>
     <t>TSO, AGC</t>
   </si>
   <si>
@@ -3501,6 +3373,30 @@
   </si>
   <si>
     <t>FrequencyControlArchi_OverviewMAESHA.png</t>
+  </si>
+  <si>
+    <t>Sc1- "Frequency reserve requirements"</t>
+  </si>
+  <si>
+    <t>Sc2- "Detection of the frequency issues - Frequency Containment Reservce (FCR)"</t>
+  </si>
+  <si>
+    <t>Sc3- "Detection of the frequency issues - Frequency Restoration Reserve (FRR)"</t>
+  </si>
+  <si>
+    <t>Sc4- "Contracting balancing service products"</t>
+  </si>
+  <si>
+    <t>Sc5- "Flexibility activation through local controller - FCR"</t>
+  </si>
+  <si>
+    <t>Sc6- "Flexibility activation through the Flexibility Management and Trading Platform - FRR"</t>
+  </si>
+  <si>
+    <t>Sc7- "Settlement process to remunerate flexibility activation"</t>
+  </si>
+  <si>
+    <t>Sc8- "Frequency control by flexibility provider"</t>
   </si>
 </sst>
 </file>
@@ -4243,8 +4139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4349,7 +4245,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>574</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -4488,7 +4384,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>575</v>
+        <v>538</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -4565,7 +4461,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>576</v>
+        <v>539</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -4577,7 +4473,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>577</v>
+        <v>540</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="19"/>
@@ -4757,22 +4653,22 @@
         <v>80</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>589</v>
+        <v>549</v>
       </c>
       <c r="D41" s="18" t="s">
-        <v>590</v>
+        <v>550</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>591</v>
+        <v>551</v>
       </c>
       <c r="F41" s="18" t="s">
-        <v>592</v>
+        <v>552</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>593</v>
+        <v>553</v>
       </c>
       <c r="H41" s="18" t="s">
-        <v>594</v>
+        <v>554</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5363,7 +5259,7 @@
         <v>119</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>587</v>
+        <v>547</v>
       </c>
       <c r="F65" s="18" t="s">
         <v>116</v>
@@ -5417,7 +5313,7 @@
         <v>60</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>588</v>
+        <v>548</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>190</v>
@@ -5540,175 +5436,175 @@
         <v>63</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>182</v>
+        <v>555</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>182</v>
+        <v>555</v>
       </c>
       <c r="E70" s="18" t="s">
-        <v>182</v>
+        <v>555</v>
       </c>
       <c r="F70" s="18" t="s">
-        <v>182</v>
+        <v>555</v>
       </c>
       <c r="G70" s="18" t="s">
-        <v>182</v>
+        <v>555</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>182</v>
+        <v>555</v>
       </c>
       <c r="I70" s="26" t="s">
-        <v>584</v>
+        <v>556</v>
       </c>
       <c r="J70" s="26" t="s">
-        <v>584</v>
+        <v>556</v>
       </c>
       <c r="K70" s="26" t="s">
-        <v>584</v>
+        <v>556</v>
       </c>
       <c r="L70" s="26" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
       <c r="M70" s="26" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
       <c r="N70" s="26" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
       <c r="O70" s="26" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
       <c r="P70" s="26" t="s">
-        <v>585</v>
+        <v>557</v>
       </c>
       <c r="Q70" s="26" t="s">
-        <v>197</v>
+        <v>558</v>
       </c>
       <c r="R70" s="26" t="s">
-        <v>197</v>
+        <v>558</v>
       </c>
       <c r="S70" s="26" t="s">
-        <v>197</v>
+        <v>558</v>
       </c>
       <c r="T70" s="26" t="s">
-        <v>197</v>
+        <v>558</v>
       </c>
       <c r="U70" s="26" t="s">
-        <v>197</v>
+        <v>558</v>
       </c>
       <c r="V70" s="26" t="s">
-        <v>197</v>
+        <v>558</v>
       </c>
       <c r="W70" s="26" t="s">
-        <v>197</v>
+        <v>558</v>
       </c>
       <c r="X70" s="26" t="s">
-        <v>203</v>
+        <v>559</v>
       </c>
       <c r="Y70" s="26" t="s">
-        <v>203</v>
+        <v>559</v>
       </c>
       <c r="Z70" s="26" t="s">
-        <v>203</v>
+        <v>559</v>
       </c>
       <c r="AA70" s="26" t="s">
-        <v>203</v>
+        <v>559</v>
       </c>
       <c r="AB70" s="26" t="s">
-        <v>203</v>
+        <v>559</v>
       </c>
       <c r="AC70" s="26" t="s">
-        <v>203</v>
+        <v>559</v>
       </c>
       <c r="AD70" s="26" t="s">
-        <v>203</v>
+        <v>559</v>
       </c>
       <c r="AE70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AF70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AG70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AH70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AI70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AJ70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AK70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AL70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AM70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AN70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AO70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AP70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AQ70" s="26" t="s">
-        <v>586</v>
+        <v>560</v>
       </c>
       <c r="AR70" s="26" t="s">
-        <v>215</v>
+        <v>561</v>
       </c>
       <c r="AS70" s="26" t="s">
-        <v>215</v>
+        <v>561</v>
       </c>
       <c r="AT70" s="26" t="s">
-        <v>215</v>
+        <v>561</v>
       </c>
       <c r="AU70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="AV70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="AW70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="AX70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="AY70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="AZ70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="BA70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="BB70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="BC70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="BD70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="BE70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="BF70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
       <c r="BG70" s="26" t="s">
-        <v>222</v>
+        <v>562</v>
       </c>
     </row>
     <row r="71" spans="1:59" x14ac:dyDescent="0.35">
@@ -5807,10 +5703,10 @@
         <v>2</v>
       </c>
       <c r="AG71" s="18" t="s">
-        <v>580</v>
+        <v>543</v>
       </c>
       <c r="AH71" s="18" t="s">
-        <v>581</v>
+        <v>544</v>
       </c>
       <c r="AI71" s="18">
         <v>4</v>
@@ -5828,10 +5724,10 @@
         <v>8</v>
       </c>
       <c r="AN71" s="18" t="s">
-        <v>582</v>
+        <v>545</v>
       </c>
       <c r="AO71" s="18" t="s">
-        <v>583</v>
+        <v>546</v>
       </c>
       <c r="AP71" s="18">
         <v>10</v>
@@ -5909,160 +5805,160 @@
         <v>227</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="I72" s="26" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="J72" s="26" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="K72" s="26" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="L72" s="26" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="M72" s="26" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="N72" s="26" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="O72" s="26" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="P72" s="26" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="Q72" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="R72" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="S72" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="R72" s="26" t="s">
+      <c r="T72" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="S72" s="26" t="s">
+      <c r="U72" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="V72" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="T72" s="26" t="s">
+      <c r="W72" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="U72" s="26" t="s">
-        <v>314</v>
-      </c>
-      <c r="V72" s="26" t="s">
-        <v>318</v>
-      </c>
-      <c r="W72" s="26" t="s">
-        <v>324</v>
-      </c>
       <c r="X72" s="26" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="Y72" s="26" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="Z72" s="26" t="s">
+        <v>321</v>
+      </c>
+      <c r="AA72" s="26" t="s">
+        <v>325</v>
+      </c>
+      <c r="AB72" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="AC72" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD72" s="26" t="s">
+        <v>336</v>
+      </c>
+      <c r="AE72" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="AA72" s="26" t="s">
+      <c r="AF72" s="26" t="s">
         <v>344</v>
       </c>
-      <c r="AB72" s="26" t="s">
-        <v>269</v>
-      </c>
-      <c r="AC72" s="26" t="s">
-        <v>354</v>
-      </c>
-      <c r="AD72" s="26" t="s">
+      <c r="AG72" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="AH72" s="26" t="s">
+        <v>353</v>
+      </c>
+      <c r="AI72" s="26" t="s">
         <v>357</v>
       </c>
-      <c r="AE72" s="26" t="s">
-        <v>360</v>
-      </c>
-      <c r="AF72" s="26" t="s">
+      <c r="AJ72" s="26" t="s">
+        <v>361</v>
+      </c>
+      <c r="AK72" s="26" t="s">
         <v>366</v>
       </c>
-      <c r="AG72" s="26" t="s">
-        <v>371</v>
-      </c>
-      <c r="AH72" s="26" t="s">
-        <v>377</v>
-      </c>
-      <c r="AI72" s="26" t="s">
+      <c r="AL72" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="AM72" s="26" t="s">
+        <v>368</v>
+      </c>
+      <c r="AN72" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="AO72" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="AP72" s="26" t="s">
+        <v>380</v>
+      </c>
+      <c r="AQ72" s="26" t="s">
         <v>382</v>
       </c>
-      <c r="AJ72" s="26" t="s">
-        <v>387</v>
-      </c>
-      <c r="AK72" s="26" t="s">
+      <c r="AR72" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="AS72" s="26" t="s">
+        <v>389</v>
+      </c>
+      <c r="AT72" s="26" t="s">
         <v>393</v>
       </c>
-      <c r="AL72" s="26" t="s">
-        <v>396</v>
-      </c>
-      <c r="AM72" s="26" t="s">
-        <v>396</v>
-      </c>
-      <c r="AN72" s="26" t="s">
-        <v>269</v>
-      </c>
-      <c r="AO72" s="26" t="s">
-        <v>409</v>
-      </c>
-      <c r="AP72" s="26" t="s">
+      <c r="AU72" s="26" t="s">
+        <v>385</v>
+      </c>
+      <c r="AV72" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="AW72" s="26" t="s">
+        <v>401</v>
+      </c>
+      <c r="AX72" s="26" t="s">
+        <v>408</v>
+      </c>
+      <c r="AY72" s="26" t="s">
         <v>412</v>
       </c>
-      <c r="AQ72" s="26" t="s">
-        <v>414</v>
-      </c>
-      <c r="AR72" s="26" t="s">
-        <v>417</v>
-      </c>
-      <c r="AS72" s="26" t="s">
-        <v>422</v>
-      </c>
-      <c r="AT72" s="26" t="s">
-        <v>426</v>
-      </c>
-      <c r="AU72" s="26" t="s">
-        <v>417</v>
-      </c>
-      <c r="AV72" s="26" t="s">
-        <v>435</v>
-      </c>
-      <c r="AW72" s="26" t="s">
-        <v>435</v>
-      </c>
-      <c r="AX72" s="26" t="s">
-        <v>443</v>
-      </c>
-      <c r="AY72" s="26" t="s">
-        <v>448</v>
-      </c>
       <c r="AZ72" s="26" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="BA72" s="26" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="BB72" s="26" t="s">
-        <v>457</v>
+        <v>421</v>
       </c>
       <c r="BC72" s="26" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="BD72" s="26" t="s">
-        <v>461</v>
+        <v>425</v>
       </c>
       <c r="BE72" s="26" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="BF72" s="26" t="s">
-        <v>465</v>
+        <v>429</v>
       </c>
       <c r="BG72" s="26" t="s">
-        <v>468</v>
+        <v>432</v>
       </c>
     </row>
     <row r="73" spans="1:59" ht="29" x14ac:dyDescent="0.35">
@@ -6074,172 +5970,172 @@
         <v>228</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F73" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G73" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="G73" s="26" t="s">
+      <c r="H73" s="18" t="s">
         <v>246</v>
       </c>
-      <c r="H73" s="18" t="s">
-        <v>251</v>
-      </c>
       <c r="I73" s="18" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="J73" s="26" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="K73" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="L73" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="M73" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="L73" s="18" t="s">
-        <v>270</v>
-      </c>
-      <c r="M73" s="18" t="s">
-        <v>274</v>
-      </c>
       <c r="N73" s="26" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="O73" s="26" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="P73" s="26" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="Q73" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="R73" s="26" t="s">
+        <v>285</v>
+      </c>
+      <c r="S73" s="26" t="s">
         <v>292</v>
       </c>
-      <c r="R73" s="26" t="s">
+      <c r="T73" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="S73" s="26" t="s">
+      <c r="U73" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="V73" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="T73" s="26" t="s">
+      <c r="W73" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="U73" s="26" t="s">
-        <v>315</v>
-      </c>
-      <c r="V73" s="26" t="s">
-        <v>319</v>
-      </c>
-      <c r="W73" s="26" t="s">
-        <v>325</v>
-      </c>
       <c r="X73" s="26" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="Y73" s="26" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="Z73" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="AA73" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="AB73" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="AC73" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="AD73" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="AE73" s="26" t="s">
         <v>340</v>
       </c>
-      <c r="AA73" s="26" t="s">
+      <c r="AF73" s="26" t="s">
         <v>345</v>
       </c>
-      <c r="AB73" s="26" t="s">
+      <c r="AG73" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="AC73" s="26" t="s">
-        <v>355</v>
-      </c>
-      <c r="AD73" s="26" t="s">
+      <c r="AH73" s="26" t="s">
+        <v>354</v>
+      </c>
+      <c r="AI73" s="26" t="s">
         <v>358</v>
       </c>
-      <c r="AE73" s="26" t="s">
-        <v>361</v>
-      </c>
-      <c r="AF73" s="26" t="s">
-        <v>367</v>
-      </c>
-      <c r="AG73" s="26" t="s">
-        <v>372</v>
-      </c>
-      <c r="AH73" s="26" t="s">
-        <v>378</v>
-      </c>
-      <c r="AI73" s="26" t="s">
-        <v>383</v>
-      </c>
       <c r="AJ73" s="26" t="s">
-        <v>388</v>
+        <v>362</v>
       </c>
       <c r="AK73" s="26" t="s">
         <v>213</v>
       </c>
       <c r="AL73" s="26" t="s">
+        <v>369</v>
+      </c>
+      <c r="AM73" s="26" t="s">
+        <v>372</v>
+      </c>
+      <c r="AN73" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="AO73" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="AP73" s="26" t="s">
+        <v>334</v>
+      </c>
+      <c r="AQ73" s="26" t="s">
+        <v>383</v>
+      </c>
+      <c r="AR73" s="26" t="s">
+        <v>386</v>
+      </c>
+      <c r="AS73" s="26" t="s">
+        <v>390</v>
+      </c>
+      <c r="AT73" s="26" t="s">
+        <v>394</v>
+      </c>
+      <c r="AU73" s="26" t="s">
         <v>397</v>
       </c>
-      <c r="AM73" s="26" t="s">
-        <v>401</v>
-      </c>
-      <c r="AN73" s="26" t="s">
-        <v>405</v>
-      </c>
-      <c r="AO73" s="26" t="s">
-        <v>405</v>
-      </c>
-      <c r="AP73" s="26" t="s">
-        <v>355</v>
-      </c>
-      <c r="AQ73" s="26" t="s">
+      <c r="AV73" s="26" t="s">
+        <v>402</v>
+      </c>
+      <c r="AW73" s="26" t="s">
+        <v>406</v>
+      </c>
+      <c r="AX73" s="26" t="s">
+        <v>409</v>
+      </c>
+      <c r="AY73" s="26" t="s">
+        <v>413</v>
+      </c>
+      <c r="AZ73" s="26" t="s">
         <v>415</v>
       </c>
-      <c r="AR73" s="26" t="s">
+      <c r="BA73" s="26" t="s">
         <v>418</v>
       </c>
-      <c r="AS73" s="26" t="s">
-        <v>423</v>
-      </c>
-      <c r="AT73" s="26" t="s">
-        <v>427</v>
-      </c>
-      <c r="AU73" s="26" t="s">
+      <c r="BB73" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="BC73" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="BD73" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="BE73" s="26" t="s">
+        <v>418</v>
+      </c>
+      <c r="BF73" s="26" t="s">
         <v>430</v>
       </c>
-      <c r="AV73" s="26" t="s">
-        <v>436</v>
-      </c>
-      <c r="AW73" s="26" t="s">
-        <v>441</v>
-      </c>
-      <c r="AX73" s="26" t="s">
-        <v>444</v>
-      </c>
-      <c r="AY73" s="26" t="s">
-        <v>449</v>
-      </c>
-      <c r="AZ73" s="26" t="s">
-        <v>451</v>
-      </c>
-      <c r="BA73" s="26" t="s">
-        <v>454</v>
-      </c>
-      <c r="BB73" s="26" t="s">
-        <v>458</v>
-      </c>
-      <c r="BC73" s="26" t="s">
-        <v>454</v>
-      </c>
-      <c r="BD73" s="26" t="s">
-        <v>462</v>
-      </c>
-      <c r="BE73" s="26" t="s">
-        <v>454</v>
-      </c>
-      <c r="BF73" s="26" t="s">
-        <v>466</v>
-      </c>
       <c r="BG73" s="26" t="s">
-        <v>469</v>
+        <v>433</v>
       </c>
     </row>
     <row r="74" spans="1:59" ht="130.5" x14ac:dyDescent="0.35">
@@ -6251,172 +6147,172 @@
         <v>229</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E74" s="26" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F74" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="G74" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="G74" s="26" t="s">
+      <c r="H74" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="H74" s="26" t="s">
-        <v>252</v>
-      </c>
       <c r="I74" s="26" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="J74" s="26" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="K74" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="L74" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="M74" s="26" t="s">
         <v>266</v>
       </c>
-      <c r="L74" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="M74" s="26" t="s">
-        <v>275</v>
-      </c>
       <c r="N74" s="26" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="O74" s="26" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="P74" s="26" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="Q74" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="R74" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="S74" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="R74" s="26" t="s">
+      <c r="T74" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="S74" s="26" t="s">
+      <c r="U74" s="26" t="s">
+        <v>302</v>
+      </c>
+      <c r="V74" s="26" t="s">
         <v>306</v>
       </c>
-      <c r="T74" s="26" t="s">
+      <c r="W74" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="U74" s="26" t="s">
-        <v>316</v>
-      </c>
-      <c r="V74" s="26" t="s">
-        <v>320</v>
-      </c>
-      <c r="W74" s="26" t="s">
-        <v>326</v>
-      </c>
       <c r="X74" s="26" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="Y74" s="26" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
       <c r="Z74" s="26" t="s">
+        <v>323</v>
+      </c>
+      <c r="AA74" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="AB74" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="AC74" s="26" t="s">
+        <v>335</v>
+      </c>
+      <c r="AD74" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="AE74" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="AA74" s="26" t="s">
+      <c r="AF74" s="26" t="s">
         <v>346</v>
       </c>
-      <c r="AB74" s="26" t="s">
+      <c r="AG74" s="26" t="s">
         <v>350</v>
       </c>
-      <c r="AC74" s="26" t="s">
-        <v>356</v>
-      </c>
-      <c r="AD74" s="26" t="s">
+      <c r="AH74" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="AI74" s="26" t="s">
         <v>359</v>
       </c>
-      <c r="AE74" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="AF74" s="26" t="s">
-        <v>368</v>
-      </c>
-      <c r="AG74" s="26" t="s">
+      <c r="AJ74" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="AK74" s="26" t="s">
+        <v>367</v>
+      </c>
+      <c r="AL74" s="26" t="s">
+        <v>370</v>
+      </c>
+      <c r="AM74" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="AH74" s="26" t="s">
+      <c r="AN74" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="AO74" s="26" t="s">
         <v>379</v>
       </c>
-      <c r="AI74" s="26" t="s">
+      <c r="AP74" s="26" t="s">
+        <v>381</v>
+      </c>
+      <c r="AQ74" s="26" t="s">
         <v>384</v>
       </c>
-      <c r="AJ74" s="26" t="s">
+      <c r="AR74" s="26" t="s">
+        <v>387</v>
+      </c>
+      <c r="AS74" s="26" t="s">
         <v>391</v>
       </c>
-      <c r="AK74" s="26" t="s">
-        <v>394</v>
-      </c>
-      <c r="AL74" s="26" t="s">
+      <c r="AT74" s="26" t="s">
+        <v>395</v>
+      </c>
+      <c r="AU74" s="26" t="s">
         <v>398</v>
       </c>
-      <c r="AM74" s="26" t="s">
-        <v>402</v>
-      </c>
-      <c r="AN74" s="26" t="s">
-        <v>406</v>
-      </c>
-      <c r="AO74" s="26" t="s">
+      <c r="AV74" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="AW74" s="26" t="s">
+        <v>407</v>
+      </c>
+      <c r="AX74" s="26" t="s">
         <v>410</v>
       </c>
-      <c r="AP74" s="26" t="s">
-        <v>413</v>
-      </c>
-      <c r="AQ74" s="26" t="s">
+      <c r="AY74" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="AZ74" s="26" t="s">
         <v>416</v>
       </c>
-      <c r="AR74" s="26" t="s">
+      <c r="BA74" s="26" t="s">
         <v>419</v>
       </c>
-      <c r="AS74" s="26" t="s">
+      <c r="BB74" s="26" t="s">
+        <v>423</v>
+      </c>
+      <c r="BC74" s="26" t="s">
         <v>424</v>
       </c>
-      <c r="AT74" s="26" t="s">
+      <c r="BD74" s="26" t="s">
+        <v>427</v>
+      </c>
+      <c r="BE74" s="26" t="s">
         <v>428</v>
       </c>
-      <c r="AU74" s="26" t="s">
+      <c r="BF74" s="26" t="s">
         <v>431</v>
       </c>
-      <c r="AV74" s="26" t="s">
-        <v>437</v>
-      </c>
-      <c r="AW74" s="26" t="s">
-        <v>442</v>
-      </c>
-      <c r="AX74" s="26" t="s">
-        <v>445</v>
-      </c>
-      <c r="AY74" s="26" t="s">
-        <v>450</v>
-      </c>
-      <c r="AZ74" s="26" t="s">
-        <v>452</v>
-      </c>
-      <c r="BA74" s="26" t="s">
-        <v>455</v>
-      </c>
-      <c r="BB74" s="26" t="s">
-        <v>459</v>
-      </c>
-      <c r="BC74" s="26" t="s">
-        <v>460</v>
-      </c>
-      <c r="BD74" s="26" t="s">
-        <v>463</v>
-      </c>
-      <c r="BE74" s="26" t="s">
-        <v>464</v>
-      </c>
-      <c r="BF74" s="26" t="s">
-        <v>467</v>
-      </c>
       <c r="BG74" s="26" t="s">
-        <v>470</v>
+        <v>434</v>
       </c>
     </row>
     <row r="75" spans="1:59" x14ac:dyDescent="0.35">
@@ -6428,7 +6324,7 @@
         <v>230</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>230</v>
@@ -6446,7 +6342,7 @@
         <v>230</v>
       </c>
       <c r="J75" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K75" s="18" t="s">
         <v>230</v>
@@ -6455,28 +6351,28 @@
         <v>230</v>
       </c>
       <c r="M75" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N75" s="18" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="O75" s="18" t="s">
         <v>230</v>
       </c>
       <c r="P75" s="18" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="Q75" s="18" t="s">
         <v>230</v>
       </c>
       <c r="R75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="S75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="T75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="U75" s="18" t="s">
         <v>230</v>
@@ -6485,7 +6381,7 @@
         <v>230</v>
       </c>
       <c r="W75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="X75" s="18" t="s">
         <v>230</v>
@@ -6494,7 +6390,7 @@
         <v>230</v>
       </c>
       <c r="Z75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AA75" s="18" t="s">
         <v>230</v>
@@ -6503,10 +6399,10 @@
         <v>230</v>
       </c>
       <c r="AC75" s="18" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="AD75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AE75" s="18" t="s">
         <v>230</v>
@@ -6515,19 +6411,19 @@
         <v>230</v>
       </c>
       <c r="AG75" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AH75" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AI75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AJ75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AK75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AL75" s="18" t="s">
         <v>230</v>
@@ -6539,22 +6435,22 @@
         <v>230</v>
       </c>
       <c r="AO75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AP75" s="18" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="AQ75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AR75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AS75" s="18" t="s">
         <v>230</v>
       </c>
       <c r="AT75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AU75" s="18" t="s">
         <v>230</v>
@@ -6569,28 +6465,28 @@
         <v>230</v>
       </c>
       <c r="AY75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="AZ75" s="18" t="s">
         <v>230</v>
       </c>
       <c r="BA75" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="BB75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="BC75" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="BD75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="BE75" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="BF75" s="18" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="BG75" s="18" t="s">
         <v>230</v>
@@ -6626,7 +6522,7 @@
         <v>154</v>
       </c>
       <c r="K76" s="18" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="L76" s="18" t="s">
         <v>154</v>
@@ -6647,10 +6543,10 @@
         <v>217</v>
       </c>
       <c r="R76" s="18" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="S76" s="18" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="T76" s="18" t="s">
         <v>217</v>
@@ -6659,22 +6555,22 @@
         <v>217</v>
       </c>
       <c r="V76" s="18" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="W76" s="18" t="s">
         <v>217</v>
       </c>
       <c r="X76" s="18" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Y76" s="18" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="Z76" s="18" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="AA76" s="18" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="AB76" s="18" t="s">
         <v>129</v>
@@ -6683,16 +6579,16 @@
         <v>217</v>
       </c>
       <c r="AD76" s="18" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="AE76" s="18" t="s">
-        <v>363</v>
+        <v>342</v>
       </c>
       <c r="AF76" s="18" t="s">
         <v>129</v>
       </c>
       <c r="AG76" s="18" t="s">
-        <v>374</v>
+        <v>351</v>
       </c>
       <c r="AH76" s="18" t="s">
         <v>139</v>
@@ -6701,13 +6597,13 @@
         <v>139</v>
       </c>
       <c r="AJ76" s="18" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
       <c r="AK76" s="18" t="s">
-        <v>342</v>
+        <v>324</v>
       </c>
       <c r="AL76" s="18" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="AM76" s="18" t="s">
         <v>131</v>
@@ -6734,43 +6630,43 @@
         <v>217</v>
       </c>
       <c r="AU76" s="18" t="s">
-        <v>432</v>
+        <v>399</v>
       </c>
       <c r="AV76" s="18" t="s">
-        <v>438</v>
+        <v>404</v>
       </c>
       <c r="AW76" s="18" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="AX76" s="18" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="AY76" s="18" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="AZ76" s="18" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="BA76" s="18" t="s">
-        <v>456</v>
+        <v>420</v>
       </c>
       <c r="BB76" s="18" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="BC76" s="18" t="s">
-        <v>456</v>
+        <v>420</v>
       </c>
       <c r="BD76" s="18" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="BE76" s="18" t="s">
-        <v>456</v>
+        <v>420</v>
       </c>
       <c r="BF76" s="18" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="BG76" s="18" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
     </row>
     <row r="77" spans="1:59" x14ac:dyDescent="0.35">
@@ -6959,325 +6855,349 @@
         <v>231</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F78" s="18" t="s">
+        <v>241</v>
+      </c>
+      <c r="G78" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="G78" s="18" t="s">
+      <c r="H78" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="H78" s="26" t="s">
-        <v>253</v>
-      </c>
       <c r="I78" s="18" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J78" s="18" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="K78" s="18" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="L78" s="18" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="M78" s="18" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="N78" s="18" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="O78" s="18" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="P78" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q78" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="R78" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="Q78" s="18" t="s">
-        <v>294</v>
-      </c>
-      <c r="R78" s="18" t="s">
-        <v>301</v>
-      </c>
       <c r="S78" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="T78" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="U78" s="26" t="s">
+        <v>303</v>
+      </c>
+      <c r="V78" s="18" t="s">
         <v>308</v>
       </c>
-      <c r="T78" s="18" t="s">
+      <c r="W78" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="U78" s="26" t="s">
-        <v>317</v>
-      </c>
-      <c r="V78" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="W78" s="18" t="s">
-        <v>327</v>
-      </c>
       <c r="X78" s="18" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y78" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z78" s="18" t="s">
+        <v>320</v>
+      </c>
+      <c r="AA78" s="18" t="s">
         <v>332</v>
       </c>
-      <c r="Y78" s="18" t="s">
-        <v>337</v>
-      </c>
-      <c r="Z78" s="18" t="s">
-        <v>337</v>
-      </c>
-      <c r="AA78" s="18" t="s">
-        <v>353</v>
-      </c>
       <c r="AB78" s="18" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="AC78" s="18" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="AD78" s="18" t="s">
-        <v>351</v>
+        <v>331</v>
       </c>
       <c r="AE78" s="18" t="s">
+        <v>343</v>
+      </c>
+      <c r="AF78" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="AG78" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="AH78" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="AI78" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="AJ78" s="26" t="s">
         <v>364</v>
       </c>
-      <c r="AF78" s="26" t="s">
-        <v>369</v>
-      </c>
-      <c r="AG78" s="18" t="s">
-        <v>375</v>
-      </c>
-      <c r="AH78" s="18" t="s">
-        <v>380</v>
-      </c>
-      <c r="AI78" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="AJ78" s="26" t="s">
-        <v>390</v>
-      </c>
       <c r="AK78" s="26" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="AL78" s="26" t="s">
-        <v>399</v>
+        <v>371</v>
       </c>
       <c r="AM78" s="26" t="s">
-        <v>403</v>
+        <v>374</v>
       </c>
       <c r="AN78" s="26" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
       <c r="AO78" s="26" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
       <c r="AP78" s="26" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
       <c r="AQ78" s="26" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
       <c r="AR78" s="26" t="s">
-        <v>420</v>
+        <v>388</v>
       </c>
       <c r="AS78" s="26" t="s">
-        <v>425</v>
+        <v>392</v>
       </c>
       <c r="AT78" s="26" t="s">
-        <v>429</v>
+        <v>396</v>
       </c>
       <c r="AU78" s="26" t="s">
-        <v>433</v>
+        <v>400</v>
       </c>
       <c r="AV78" s="26" t="s">
-        <v>439</v>
+        <v>405</v>
       </c>
       <c r="AW78" s="26" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="AX78" s="26" t="s">
-        <v>446</v>
+        <v>411</v>
       </c>
       <c r="AY78" s="26" t="s">
-        <v>446</v>
+        <v>411</v>
       </c>
       <c r="AZ78" s="26" t="s">
-        <v>453</v>
+        <v>417</v>
       </c>
       <c r="BA78" s="26" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="BB78" s="26" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="BC78" s="26" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="BD78" s="26" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="BE78" s="26" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="BF78" s="26" t="s">
-        <v>390</v>
+        <v>364</v>
       </c>
       <c r="BG78" s="26" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="79" spans="1:59" ht="43.5" x14ac:dyDescent="0.35">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="79" spans="1:59" x14ac:dyDescent="0.35">
       <c r="A79" s="12"/>
       <c r="B79" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>232</v>
+        <v>181</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>237</v>
-      </c>
-      <c r="E79" s="26" t="s">
-        <v>241</v>
+        <v>181</v>
+      </c>
+      <c r="E79" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="F79" s="18" t="s">
-        <v>245</v>
+        <v>181</v>
       </c>
       <c r="G79" s="18" t="s">
-        <v>249</v>
+        <v>181</v>
       </c>
       <c r="H79" s="18" t="s">
-        <v>254</v>
+        <v>181</v>
       </c>
       <c r="I79" s="18" t="s">
-        <v>259</v>
+        <v>186</v>
       </c>
       <c r="J79" s="18" t="s">
-        <v>263</v>
+        <v>186</v>
       </c>
       <c r="K79" s="18" t="s">
-        <v>259</v>
+        <v>186</v>
       </c>
       <c r="L79" s="18" t="s">
-        <v>273</v>
+        <v>192</v>
       </c>
       <c r="M79" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="N79" s="26" t="s">
-        <v>281</v>
+        <v>192</v>
+      </c>
+      <c r="N79" s="18" t="s">
+        <v>192</v>
       </c>
       <c r="O79" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="P79" s="26" t="s">
-        <v>290</v>
+        <v>192</v>
+      </c>
+      <c r="P79" s="18" t="s">
+        <v>192</v>
       </c>
       <c r="Q79" s="26" t="s">
-        <v>295</v>
+        <v>196</v>
       </c>
       <c r="R79" s="26" t="s">
-        <v>303</v>
+        <v>196</v>
       </c>
       <c r="S79" s="26" t="s">
-        <v>303</v>
+        <v>196</v>
       </c>
       <c r="T79" s="26" t="s">
-        <v>313</v>
+        <v>196</v>
       </c>
       <c r="U79" s="26" t="s">
-        <v>295</v>
+        <v>196</v>
       </c>
       <c r="V79" s="26" t="s">
-        <v>323</v>
+        <v>196</v>
       </c>
       <c r="W79" s="26" t="s">
-        <v>328</v>
+        <v>196</v>
       </c>
       <c r="X79" s="26" t="s">
-        <v>333</v>
+        <v>202</v>
       </c>
       <c r="Y79" s="26" t="s">
-        <v>338</v>
+        <v>202</v>
       </c>
       <c r="Z79" s="26" t="s">
-        <v>343</v>
+        <v>202</v>
       </c>
       <c r="AA79" s="26" t="s">
-        <v>348</v>
+        <v>202</v>
       </c>
       <c r="AB79" s="26" t="s">
-        <v>352</v>
-      </c>
-      <c r="AC79" s="26"/>
-      <c r="AD79" s="26"/>
+        <v>202</v>
+      </c>
+      <c r="AC79" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD79" s="26" t="s">
+        <v>202</v>
+      </c>
       <c r="AE79" s="26" t="s">
-        <v>365</v>
+        <v>208</v>
       </c>
       <c r="AF79" s="26" t="s">
-        <v>370</v>
+        <v>208</v>
       </c>
       <c r="AG79" s="26" t="s">
-        <v>376</v>
+        <v>208</v>
       </c>
       <c r="AH79" s="26" t="s">
-        <v>381</v>
+        <v>208</v>
       </c>
       <c r="AI79" s="26" t="s">
-        <v>386</v>
+        <v>208</v>
       </c>
       <c r="AJ79" s="26" t="s">
-        <v>392</v>
+        <v>208</v>
       </c>
       <c r="AK79" s="26" t="s">
-        <v>395</v>
+        <v>208</v>
       </c>
       <c r="AL79" s="26" t="s">
-        <v>400</v>
+        <v>208</v>
       </c>
       <c r="AM79" s="26" t="s">
-        <v>404</v>
+        <v>208</v>
       </c>
       <c r="AN79" s="26" t="s">
-        <v>408</v>
+        <v>208</v>
       </c>
       <c r="AO79" s="26" t="s">
-        <v>411</v>
-      </c>
-      <c r="AP79" s="26"/>
-      <c r="AQ79" s="26"/>
+        <v>208</v>
+      </c>
+      <c r="AP79" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="AQ79" s="26" t="s">
+        <v>208</v>
+      </c>
       <c r="AR79" s="26" t="s">
-        <v>421</v>
+        <v>214</v>
       </c>
       <c r="AS79" s="26" t="s">
-        <v>327</v>
+        <v>214</v>
       </c>
       <c r="AT79" s="26" t="s">
-        <v>425</v>
+        <v>214</v>
       </c>
       <c r="AU79" s="26" t="s">
-        <v>434</v>
+        <v>221</v>
       </c>
       <c r="AV79" s="26" t="s">
-        <v>440</v>
-      </c>
-      <c r="AW79" s="26"/>
+        <v>221</v>
+      </c>
+      <c r="AW79" s="26" t="s">
+        <v>221</v>
+      </c>
       <c r="AX79" s="26" t="s">
-        <v>447</v>
-      </c>
-      <c r="AY79" s="26"/>
+        <v>221</v>
+      </c>
+      <c r="AY79" s="26" t="s">
+        <v>221</v>
+      </c>
       <c r="AZ79" s="26" t="s">
-        <v>447</v>
-      </c>
-      <c r="BA79" s="26"/>
-      <c r="BB79" s="26"/>
-      <c r="BC79" s="26"/>
-      <c r="BD79" s="26"/>
-      <c r="BE79" s="26"/>
-      <c r="BF79" s="26"/>
+        <v>221</v>
+      </c>
+      <c r="BA79" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="BB79" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="BC79" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="BD79" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="BE79" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="BF79" s="26" t="s">
+        <v>221</v>
+      </c>
       <c r="BG79" s="26" t="s">
-        <v>472</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7369,112 +7289,112 @@
         <v>74</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>473</v>
+        <v>436</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>476</v>
+        <v>439</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>479</v>
+        <v>442</v>
       </c>
       <c r="F82" s="18" t="s">
-        <v>482</v>
+        <v>445</v>
       </c>
       <c r="G82" s="18" t="s">
-        <v>485</v>
+        <v>448</v>
       </c>
       <c r="H82" s="18" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>491</v>
+        <v>454</v>
       </c>
       <c r="J82" s="18" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
       <c r="K82" s="18" t="s">
-        <v>496</v>
+        <v>459</v>
       </c>
       <c r="L82" s="18" t="s">
-        <v>499</v>
+        <v>462</v>
       </c>
       <c r="M82" s="18" t="s">
-        <v>503</v>
+        <v>466</v>
       </c>
       <c r="N82" s="18" t="s">
-        <v>505</v>
+        <v>468</v>
       </c>
       <c r="O82" s="18" t="s">
+        <v>470</v>
+      </c>
+      <c r="P82" s="18" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q82" s="18" t="s">
+        <v>475</v>
+      </c>
+      <c r="R82" s="18" t="s">
+        <v>477</v>
+      </c>
+      <c r="S82" s="18" t="s">
+        <v>481</v>
+      </c>
+      <c r="T82" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="U82" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="V82" s="18" t="s">
+        <v>490</v>
+      </c>
+      <c r="W82" s="18" t="s">
+        <v>493</v>
+      </c>
+      <c r="X82" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="Y82" s="18" t="s">
+        <v>498</v>
+      </c>
+      <c r="Z82" s="18" t="s">
+        <v>501</v>
+      </c>
+      <c r="AA82" s="18" t="s">
+        <v>504</v>
+      </c>
+      <c r="AB82" s="18" t="s">
         <v>507</v>
       </c>
-      <c r="P82" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="Q82" s="18" t="s">
-        <v>512</v>
-      </c>
-      <c r="R82" s="18" t="s">
-        <v>514</v>
-      </c>
-      <c r="S82" s="18" t="s">
+      <c r="AC82" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="AD82" s="18" t="s">
+        <v>513</v>
+      </c>
+      <c r="AE82" s="18" t="s">
+        <v>515</v>
+      </c>
+      <c r="AF82" s="18" t="s">
         <v>518</v>
       </c>
-      <c r="T82" s="18" t="s">
+      <c r="AG82" s="18" t="s">
         <v>520</v>
       </c>
-      <c r="U82" s="18" t="s">
-        <v>524</v>
-      </c>
-      <c r="V82" s="18" t="s">
-        <v>527</v>
-      </c>
-      <c r="W82" s="18" t="s">
-        <v>530</v>
-      </c>
-      <c r="X82" s="18" t="s">
-        <v>532</v>
-      </c>
-      <c r="Y82" s="18" t="s">
-        <v>535</v>
-      </c>
-      <c r="Z82" s="18" t="s">
-        <v>538</v>
-      </c>
-      <c r="AA82" s="18" t="s">
-        <v>541</v>
-      </c>
-      <c r="AB82" s="18" t="s">
-        <v>544</v>
-      </c>
-      <c r="AC82" s="18" t="s">
-        <v>547</v>
-      </c>
-      <c r="AD82" s="18" t="s">
-        <v>550</v>
-      </c>
-      <c r="AE82" s="18" t="s">
-        <v>552</v>
-      </c>
-      <c r="AF82" s="18" t="s">
-        <v>555</v>
-      </c>
-      <c r="AG82" s="18" t="s">
-        <v>557</v>
-      </c>
       <c r="AH82" s="18" t="s">
-        <v>559</v>
+        <v>522</v>
       </c>
       <c r="AI82" s="18" t="s">
-        <v>562</v>
+        <v>525</v>
       </c>
       <c r="AJ82" s="18" t="s">
-        <v>565</v>
+        <v>528</v>
       </c>
       <c r="AK82" s="18" t="s">
-        <v>568</v>
+        <v>531</v>
       </c>
       <c r="AL82" s="18" t="s">
-        <v>571</v>
+        <v>534</v>
       </c>
     </row>
     <row r="83" spans="1:38" x14ac:dyDescent="0.35">
@@ -7483,112 +7403,112 @@
         <v>75</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>474</v>
+        <v>437</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>477</v>
+        <v>440</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>480</v>
+        <v>443</v>
       </c>
       <c r="F83" s="18" t="s">
-        <v>483</v>
+        <v>446</v>
       </c>
       <c r="G83" s="18" t="s">
-        <v>486</v>
+        <v>449</v>
       </c>
       <c r="H83" s="18" t="s">
-        <v>489</v>
+        <v>452</v>
       </c>
       <c r="I83" s="18" t="s">
-        <v>492</v>
+        <v>455</v>
       </c>
       <c r="J83" s="18" t="s">
-        <v>494</v>
+        <v>457</v>
       </c>
       <c r="K83" s="18" t="s">
-        <v>497</v>
+        <v>460</v>
       </c>
       <c r="L83" s="18" t="s">
-        <v>500</v>
+        <v>463</v>
       </c>
       <c r="M83" s="18" t="s">
+        <v>465</v>
+      </c>
+      <c r="N83" s="18" t="s">
+        <v>463</v>
+      </c>
+      <c r="O83" s="18" t="s">
+        <v>471</v>
+      </c>
+      <c r="P83" s="18" t="s">
+        <v>473</v>
+      </c>
+      <c r="Q83" s="18" t="s">
+        <v>479</v>
+      </c>
+      <c r="R83" s="18" t="s">
+        <v>478</v>
+      </c>
+      <c r="S83" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="T83" s="18" t="s">
+        <v>485</v>
+      </c>
+      <c r="U83" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="V83" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="W83" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="X83" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y83" s="18" t="s">
+        <v>499</v>
+      </c>
+      <c r="Z83" s="18" t="s">
         <v>502</v>
       </c>
-      <c r="N83" s="18" t="s">
-        <v>500</v>
-      </c>
-      <c r="O83" s="18" t="s">
+      <c r="AA83" s="18" t="s">
+        <v>505</v>
+      </c>
+      <c r="AB83" s="18" t="s">
         <v>508</v>
       </c>
-      <c r="P83" s="18" t="s">
-        <v>510</v>
-      </c>
-      <c r="Q83" s="18" t="s">
+      <c r="AC83" s="18" t="s">
+        <v>511</v>
+      </c>
+      <c r="AD83" s="18" t="s">
+        <v>514</v>
+      </c>
+      <c r="AE83" s="18" t="s">
         <v>516</v>
       </c>
-      <c r="R83" s="18" t="s">
-        <v>515</v>
-      </c>
-      <c r="S83" s="18" t="s">
+      <c r="AF83" s="18" t="s">
+        <v>519</v>
+      </c>
+      <c r="AG83" s="18" t="s">
         <v>521</v>
       </c>
-      <c r="T83" s="18" t="s">
-        <v>522</v>
-      </c>
-      <c r="U83" s="18" t="s">
-        <v>525</v>
-      </c>
-      <c r="V83" s="18" t="s">
-        <v>528</v>
-      </c>
-      <c r="W83" s="18" t="s">
-        <v>334</v>
-      </c>
-      <c r="X83" s="18" t="s">
-        <v>533</v>
-      </c>
-      <c r="Y83" s="18" t="s">
-        <v>536</v>
-      </c>
-      <c r="Z83" s="18" t="s">
-        <v>539</v>
-      </c>
-      <c r="AA83" s="18" t="s">
-        <v>542</v>
-      </c>
-      <c r="AB83" s="18" t="s">
-        <v>545</v>
-      </c>
-      <c r="AC83" s="18" t="s">
-        <v>548</v>
-      </c>
-      <c r="AD83" s="18" t="s">
-        <v>551</v>
-      </c>
-      <c r="AE83" s="18" t="s">
-        <v>553</v>
-      </c>
-      <c r="AF83" s="18" t="s">
-        <v>556</v>
-      </c>
-      <c r="AG83" s="18" t="s">
-        <v>558</v>
-      </c>
       <c r="AH83" s="18" t="s">
-        <v>560</v>
+        <v>523</v>
       </c>
       <c r="AI83" s="18" t="s">
-        <v>563</v>
+        <v>526</v>
       </c>
       <c r="AJ83" s="18" t="s">
-        <v>566</v>
+        <v>529</v>
       </c>
       <c r="AK83" s="18" t="s">
-        <v>569</v>
+        <v>532</v>
       </c>
       <c r="AL83" s="18" t="s">
-        <v>572</v>
+        <v>535</v>
       </c>
     </row>
     <row r="84" spans="1:38" ht="72.5" x14ac:dyDescent="0.35">
@@ -7597,110 +7517,110 @@
         <v>76</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>475</v>
+        <v>438</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>478</v>
+        <v>441</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>481</v>
+        <v>444</v>
       </c>
       <c r="F84" s="26" t="s">
-        <v>484</v>
+        <v>447</v>
       </c>
       <c r="G84" s="26" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="H84" s="26" t="s">
-        <v>490</v>
+        <v>453</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>493</v>
+        <v>456</v>
       </c>
       <c r="J84" s="26" t="s">
-        <v>495</v>
+        <v>458</v>
       </c>
       <c r="K84" s="26" t="s">
-        <v>498</v>
+        <v>461</v>
       </c>
       <c r="L84" s="26" t="s">
-        <v>501</v>
+        <v>464</v>
       </c>
       <c r="M84" s="26" t="s">
-        <v>504</v>
+        <v>467</v>
       </c>
       <c r="N84" s="26" t="s">
+        <v>469</v>
+      </c>
+      <c r="O84" s="26" t="s">
+        <v>472</v>
+      </c>
+      <c r="P84" s="26" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q84" s="26" t="s">
+        <v>476</v>
+      </c>
+      <c r="R84" s="26" t="s">
+        <v>480</v>
+      </c>
+      <c r="S84" s="26" t="s">
+        <v>482</v>
+      </c>
+      <c r="T84" s="26" t="s">
+        <v>486</v>
+      </c>
+      <c r="U84" s="26" t="s">
+        <v>489</v>
+      </c>
+      <c r="V84" s="26" t="s">
+        <v>492</v>
+      </c>
+      <c r="W84" s="26" t="s">
+        <v>494</v>
+      </c>
+      <c r="X84" s="26" t="s">
+        <v>497</v>
+      </c>
+      <c r="Y84" s="26" t="s">
+        <v>500</v>
+      </c>
+      <c r="Z84" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="AA84" s="26" t="s">
         <v>506</v>
       </c>
-      <c r="O84" s="26" t="s">
+      <c r="AB84" s="26" t="s">
         <v>509</v>
       </c>
-      <c r="P84" s="26" t="s">
-        <v>511</v>
-      </c>
-      <c r="Q84" s="26" t="s">
-        <v>513</v>
-      </c>
-      <c r="R84" s="26" t="s">
-        <v>517</v>
-      </c>
-      <c r="S84" s="26" t="s">
-        <v>519</v>
-      </c>
-      <c r="T84" s="26" t="s">
-        <v>523</v>
-      </c>
-      <c r="U84" s="26" t="s">
-        <v>526</v>
-      </c>
-      <c r="V84" s="26" t="s">
-        <v>529</v>
-      </c>
-      <c r="W84" s="26" t="s">
-        <v>531</v>
-      </c>
-      <c r="X84" s="26" t="s">
-        <v>534</v>
-      </c>
-      <c r="Y84" s="26" t="s">
-        <v>537</v>
-      </c>
-      <c r="Z84" s="26" t="s">
-        <v>540</v>
-      </c>
-      <c r="AA84" s="26" t="s">
-        <v>543</v>
-      </c>
-      <c r="AB84" s="26" t="s">
-        <v>546</v>
-      </c>
       <c r="AC84" s="26" t="s">
-        <v>549</v>
+        <v>512</v>
       </c>
       <c r="AD84" s="26"/>
       <c r="AE84" s="26" t="s">
-        <v>554</v>
+        <v>517</v>
       </c>
       <c r="AF84" s="26" t="s">
-        <v>578</v>
+        <v>541</v>
       </c>
       <c r="AG84" s="26" t="s">
-        <v>579</v>
+        <v>542</v>
       </c>
       <c r="AH84" s="26" t="s">
-        <v>561</v>
+        <v>524</v>
       </c>
       <c r="AI84" s="26" t="s">
-        <v>564</v>
+        <v>527</v>
       </c>
       <c r="AJ84" s="26" t="s">
-        <v>567</v>
+        <v>530</v>
       </c>
       <c r="AK84" s="26" t="s">
-        <v>570</v>
+        <v>533</v>
       </c>
       <c r="AL84" s="26" t="s">
-        <v>573</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test primary actor of scenario & Info exchanged ID
</commit_message>
<xml_diff>
--- a/excel-use-cases/MAESHA/IEC62559-2_TEMPLATE_FrequencyControlUC.xlsx
+++ b/excel-use-cases/MAESHA/IEC62559-2_TEMPLATE_FrequencyControlUC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MAESHA\08_BRIDGE\Data Management WG\UC repository\MAESHA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3AC089-06B8-4A17-A9FC-0BE4304463C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F469A2-ED0D-48F9-87FD-D90F00C5C790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IEC62559-2" sheetId="1" r:id="rId1"/>
@@ -1363,7 +1363,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="565">
   <si>
     <t>1 Description of the use case</t>
   </si>
@@ -2059,9 +2059,6 @@
   </si>
   <si>
     <t>CREATE</t>
-  </si>
-  <si>
-    <t>IE-01-01 (frequency bandwigth and emergency thresholds)</t>
   </si>
   <si>
     <t>Collect data of the power system</t>
@@ -3397,6 +3394,15 @@
   </si>
   <si>
     <t>Sc8- "Frequency control by flexibility provider"</t>
+  </si>
+  <si>
+    <t>"TSO"</t>
+  </si>
+  <si>
+    <t>"Flexibility provider"</t>
+  </si>
+  <si>
+    <t>"IE-01-01"</t>
   </si>
 </sst>
 </file>
@@ -4139,8 +4145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="B78" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4245,7 +4251,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -4384,7 +4390,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -4461,7 +4467,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -4473,7 +4479,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="19"/>
@@ -4653,22 +4659,22 @@
         <v>80</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="D41" s="18" t="s">
         <v>549</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="E41" s="18" t="s">
         <v>550</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="F41" s="18" t="s">
         <v>551</v>
       </c>
-      <c r="F41" s="18" t="s">
+      <c r="G41" s="18" t="s">
         <v>552</v>
       </c>
-      <c r="G41" s="18" t="s">
+      <c r="H41" s="18" t="s">
         <v>553</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="42" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -5253,13 +5259,13 @@
         <v>58</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>116</v>
+        <v>562</v>
       </c>
       <c r="D65" s="18" t="s">
-        <v>119</v>
+        <v>563</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F65" s="18" t="s">
         <v>116</v>
@@ -5313,7 +5319,7 @@
         <v>60</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D67" s="18" t="s">
         <v>190</v>
@@ -5436,175 +5442,175 @@
         <v>63</v>
       </c>
       <c r="C70" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>554</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>554</v>
+      </c>
+      <c r="F70" s="18" t="s">
+        <v>554</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>554</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>554</v>
+      </c>
+      <c r="I70" s="26" t="s">
         <v>555</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="J70" s="26" t="s">
         <v>555</v>
       </c>
-      <c r="E70" s="18" t="s">
+      <c r="K70" s="26" t="s">
         <v>555</v>
       </c>
-      <c r="F70" s="18" t="s">
-        <v>555</v>
-      </c>
-      <c r="G70" s="18" t="s">
-        <v>555</v>
-      </c>
-      <c r="H70" s="18" t="s">
-        <v>555</v>
-      </c>
-      <c r="I70" s="26" t="s">
+      <c r="L70" s="26" t="s">
         <v>556</v>
       </c>
-      <c r="J70" s="26" t="s">
+      <c r="M70" s="26" t="s">
         <v>556</v>
       </c>
-      <c r="K70" s="26" t="s">
+      <c r="N70" s="26" t="s">
         <v>556</v>
       </c>
-      <c r="L70" s="26" t="s">
+      <c r="O70" s="26" t="s">
+        <v>556</v>
+      </c>
+      <c r="P70" s="26" t="s">
+        <v>556</v>
+      </c>
+      <c r="Q70" s="26" t="s">
         <v>557</v>
       </c>
-      <c r="M70" s="26" t="s">
+      <c r="R70" s="26" t="s">
         <v>557</v>
       </c>
-      <c r="N70" s="26" t="s">
+      <c r="S70" s="26" t="s">
         <v>557</v>
       </c>
-      <c r="O70" s="26" t="s">
+      <c r="T70" s="26" t="s">
         <v>557</v>
       </c>
-      <c r="P70" s="26" t="s">
+      <c r="U70" s="26" t="s">
         <v>557</v>
       </c>
-      <c r="Q70" s="26" t="s">
+      <c r="V70" s="26" t="s">
+        <v>557</v>
+      </c>
+      <c r="W70" s="26" t="s">
+        <v>557</v>
+      </c>
+      <c r="X70" s="26" t="s">
         <v>558</v>
       </c>
-      <c r="R70" s="26" t="s">
+      <c r="Y70" s="26" t="s">
         <v>558</v>
       </c>
-      <c r="S70" s="26" t="s">
+      <c r="Z70" s="26" t="s">
         <v>558</v>
       </c>
-      <c r="T70" s="26" t="s">
+      <c r="AA70" s="26" t="s">
         <v>558</v>
       </c>
-      <c r="U70" s="26" t="s">
+      <c r="AB70" s="26" t="s">
         <v>558</v>
       </c>
-      <c r="V70" s="26" t="s">
+      <c r="AC70" s="26" t="s">
         <v>558</v>
       </c>
-      <c r="W70" s="26" t="s">
+      <c r="AD70" s="26" t="s">
         <v>558</v>
       </c>
-      <c r="X70" s="26" t="s">
+      <c r="AE70" s="26" t="s">
         <v>559</v>
       </c>
-      <c r="Y70" s="26" t="s">
+      <c r="AF70" s="26" t="s">
         <v>559</v>
       </c>
-      <c r="Z70" s="26" t="s">
+      <c r="AG70" s="26" t="s">
         <v>559</v>
       </c>
-      <c r="AA70" s="26" t="s">
+      <c r="AH70" s="26" t="s">
         <v>559</v>
       </c>
-      <c r="AB70" s="26" t="s">
+      <c r="AI70" s="26" t="s">
         <v>559</v>
       </c>
-      <c r="AC70" s="26" t="s">
+      <c r="AJ70" s="26" t="s">
         <v>559</v>
       </c>
-      <c r="AD70" s="26" t="s">
+      <c r="AK70" s="26" t="s">
         <v>559</v>
       </c>
-      <c r="AE70" s="26" t="s">
+      <c r="AL70" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="AM70" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="AN70" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="AO70" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="AP70" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="AQ70" s="26" t="s">
+        <v>559</v>
+      </c>
+      <c r="AR70" s="26" t="s">
         <v>560</v>
       </c>
-      <c r="AF70" s="26" t="s">
+      <c r="AS70" s="26" t="s">
         <v>560</v>
       </c>
-      <c r="AG70" s="26" t="s">
+      <c r="AT70" s="26" t="s">
         <v>560</v>
       </c>
-      <c r="AH70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AI70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AJ70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AK70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AL70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AM70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AN70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AO70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AP70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AQ70" s="26" t="s">
-        <v>560</v>
-      </c>
-      <c r="AR70" s="26" t="s">
+      <c r="AU70" s="26" t="s">
         <v>561</v>
       </c>
-      <c r="AS70" s="26" t="s">
+      <c r="AV70" s="26" t="s">
         <v>561</v>
       </c>
-      <c r="AT70" s="26" t="s">
+      <c r="AW70" s="26" t="s">
         <v>561</v>
       </c>
-      <c r="AU70" s="26" t="s">
-        <v>562</v>
-      </c>
-      <c r="AV70" s="26" t="s">
-        <v>562</v>
-      </c>
-      <c r="AW70" s="26" t="s">
-        <v>562</v>
-      </c>
       <c r="AX70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AY70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="AZ70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="BA70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="BB70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="BC70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="BD70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="BE70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="BF70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="BG70" s="26" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="71" spans="1:59" x14ac:dyDescent="0.35">
@@ -5703,10 +5709,10 @@
         <v>2</v>
       </c>
       <c r="AG71" s="18" t="s">
+        <v>542</v>
+      </c>
+      <c r="AH71" s="18" t="s">
         <v>543</v>
-      </c>
-      <c r="AH71" s="18" t="s">
-        <v>544</v>
       </c>
       <c r="AI71" s="18">
         <v>4</v>
@@ -5724,10 +5730,10 @@
         <v>8</v>
       </c>
       <c r="AN71" s="18" t="s">
+        <v>544</v>
+      </c>
+      <c r="AO71" s="18" t="s">
         <v>545</v>
-      </c>
-      <c r="AO71" s="18" t="s">
-        <v>546</v>
       </c>
       <c r="AP71" s="18">
         <v>10</v>
@@ -5805,160 +5811,160 @@
         <v>227</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I72" s="26" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J72" s="26" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K72" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L72" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M72" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="N72" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O72" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P72" s="26" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="Q72" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R72" s="26" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="S72" s="26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="T72" s="26" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="U72" s="26" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="V72" s="26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="W72" s="26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="X72" s="26" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Y72" s="26" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Z72" s="26" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="AA72" s="26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="AB72" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AC72" s="26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="AD72" s="26" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AE72" s="26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AF72" s="26" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AG72" s="26" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AH72" s="26" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AI72" s="26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AJ72" s="26" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="AK72" s="26" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="AL72" s="26" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AM72" s="26" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="AN72" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AO72" s="26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AP72" s="26" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="AQ72" s="26" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="AR72" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AS72" s="26" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AT72" s="26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AU72" s="26" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AV72" s="26" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AW72" s="26" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="AX72" s="26" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AY72" s="26" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AZ72" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BA72" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BB72" s="26" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="BC72" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BD72" s="26" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="BE72" s="26" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BF72" s="26" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="BG72" s="26" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="73" spans="1:59" ht="29" x14ac:dyDescent="0.35">
@@ -5970,172 +5976,172 @@
         <v>228</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E73" s="18" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F73" s="18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G73" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I73" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J73" s="26" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K73" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L73" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M73" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="N73" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O73" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="P73" s="26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q73" s="26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="R73" s="26" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="S73" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="T73" s="26" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="U73" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="V73" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="W73" s="26" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="X73" s="26" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Y73" s="26" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Z73" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AA73" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AB73" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AC73" s="26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AD73" s="26" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AE73" s="26" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AF73" s="26" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AG73" s="26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AH73" s="26" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AI73" s="26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AJ73" s="26" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AK73" s="26" t="s">
         <v>213</v>
       </c>
       <c r="AL73" s="26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="AM73" s="26" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="AN73" s="26" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AO73" s="26" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="AP73" s="26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="AQ73" s="26" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="AR73" s="26" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="AS73" s="26" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="AT73" s="26" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AU73" s="26" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AV73" s="26" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AW73" s="26" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AX73" s="26" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AY73" s="26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AZ73" s="26" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="BA73" s="26" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="BB73" s="26" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="BC73" s="26" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="BD73" s="26" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="BE73" s="26" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="BF73" s="26" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="BG73" s="26" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="74" spans="1:59" ht="130.5" x14ac:dyDescent="0.35">
@@ -6147,172 +6153,172 @@
         <v>229</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E74" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F74" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G74" s="26" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H74" s="26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I74" s="26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J74" s="26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K74" s="26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="L74" s="26" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M74" s="26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N74" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O74" s="26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P74" s="26" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="Q74" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="R74" s="26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="S74" s="26" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="T74" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="U74" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="V74" s="26" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="W74" s="26" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="X74" s="26" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Y74" s="26" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Z74" s="26" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AA74" s="26" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AB74" s="26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AC74" s="26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AD74" s="26" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AE74" s="26" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AF74" s="26" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AG74" s="26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AH74" s="26" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AI74" s="26" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="AJ74" s="26" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="AK74" s="26" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="AL74" s="26" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AM74" s="26" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="AN74" s="26" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="AO74" s="26" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="AP74" s="26" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="AQ74" s="26" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="AR74" s="26" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AS74" s="26" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AT74" s="26" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AU74" s="26" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AV74" s="26" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AW74" s="26" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AX74" s="26" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AY74" s="26" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="AZ74" s="26" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="BA74" s="26" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="BB74" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="BC74" s="26" t="s">
         <v>423</v>
       </c>
-      <c r="BC74" s="26" t="s">
-        <v>424</v>
-      </c>
       <c r="BD74" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="BE74" s="26" t="s">
         <v>427</v>
       </c>
-      <c r="BE74" s="26" t="s">
-        <v>428</v>
-      </c>
       <c r="BF74" s="26" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="BG74" s="26" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="75" spans="1:59" x14ac:dyDescent="0.35">
@@ -6324,7 +6330,7 @@
         <v>230</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>230</v>
@@ -6342,7 +6348,7 @@
         <v>230</v>
       </c>
       <c r="J75" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K75" s="18" t="s">
         <v>230</v>
@@ -6351,28 +6357,28 @@
         <v>230</v>
       </c>
       <c r="M75" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="N75" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O75" s="18" t="s">
         <v>230</v>
       </c>
       <c r="P75" s="18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="Q75" s="18" t="s">
         <v>230</v>
       </c>
       <c r="R75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="S75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="T75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="U75" s="18" t="s">
         <v>230</v>
@@ -6381,7 +6387,7 @@
         <v>230</v>
       </c>
       <c r="W75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="X75" s="18" t="s">
         <v>230</v>
@@ -6390,7 +6396,7 @@
         <v>230</v>
       </c>
       <c r="Z75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AA75" s="18" t="s">
         <v>230</v>
@@ -6399,10 +6405,10 @@
         <v>230</v>
       </c>
       <c r="AC75" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AD75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AE75" s="18" t="s">
         <v>230</v>
@@ -6411,19 +6417,19 @@
         <v>230</v>
       </c>
       <c r="AG75" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AH75" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AI75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AJ75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AK75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AL75" s="18" t="s">
         <v>230</v>
@@ -6435,22 +6441,22 @@
         <v>230</v>
       </c>
       <c r="AO75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AP75" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AQ75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AR75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AS75" s="18" t="s">
         <v>230</v>
       </c>
       <c r="AT75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AU75" s="18" t="s">
         <v>230</v>
@@ -6465,28 +6471,28 @@
         <v>230</v>
       </c>
       <c r="AY75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="AZ75" s="18" t="s">
         <v>230</v>
       </c>
       <c r="BA75" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BB75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="BC75" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BD75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="BE75" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BF75" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="BG75" s="18" t="s">
         <v>230</v>
@@ -6522,7 +6528,7 @@
         <v>154</v>
       </c>
       <c r="K76" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="L76" s="18" t="s">
         <v>154</v>
@@ -6543,10 +6549,10 @@
         <v>217</v>
       </c>
       <c r="R76" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S76" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="T76" s="18" t="s">
         <v>217</v>
@@ -6555,22 +6561,22 @@
         <v>217</v>
       </c>
       <c r="V76" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="W76" s="18" t="s">
         <v>217</v>
       </c>
       <c r="X76" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Y76" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Z76" s="18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AA76" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AB76" s="18" t="s">
         <v>129</v>
@@ -6579,16 +6585,16 @@
         <v>217</v>
       </c>
       <c r="AD76" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="AE76" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AF76" s="18" t="s">
         <v>129</v>
       </c>
       <c r="AG76" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AH76" s="18" t="s">
         <v>139</v>
@@ -6597,13 +6603,13 @@
         <v>139</v>
       </c>
       <c r="AJ76" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="AK76" s="18" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="AL76" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AM76" s="18" t="s">
         <v>131</v>
@@ -6630,43 +6636,43 @@
         <v>217</v>
       </c>
       <c r="AU76" s="18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="AV76" s="18" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AW76" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AX76" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AY76" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="AZ76" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="BA76" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="BB76" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="BC76" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="BD76" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="BE76" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="BF76" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="BG76" s="18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="77" spans="1:59" x14ac:dyDescent="0.35">
@@ -6852,175 +6858,175 @@
         <v>71</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>231</v>
+        <v>564</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E78" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F78" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G78" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H78" s="26" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I78" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J78" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K78" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="L78" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M78" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N78" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O78" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P78" s="18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Q78" s="18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="R78" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="S78" s="26" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="T78" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="U78" s="26" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="V78" s="18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="W78" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="X78" s="18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Y78" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Z78" s="18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AA78" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AB78" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AC78" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AD78" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AE78" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AF78" s="26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="AG78" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AH78" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AI78" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AJ78" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AK78" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="AL78" s="26" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="AM78" s="26" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AN78" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AO78" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AP78" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AQ78" s="26" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="AR78" s="26" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AS78" s="26" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="AT78" s="26" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AU78" s="26" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AV78" s="26" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AW78" s="26" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AX78" s="26" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AY78" s="26" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="AZ78" s="26" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="BA78" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="BB78" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="BC78" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="BD78" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="BE78" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="BF78" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="BG78" s="26" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="79" spans="1:59" x14ac:dyDescent="0.35">
@@ -7289,112 +7295,112 @@
         <v>74</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E82" s="18" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F82" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G82" s="18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H82" s="18" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I82" s="18" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J82" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K82" s="18" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="L82" s="18" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="M82" s="18" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="N82" s="18" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="O82" s="18" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="P82" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="Q82" s="18" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="R82" s="18" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="S82" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="T82" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="U82" s="18" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="V82" s="18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="W82" s="18" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="X82" s="18" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Y82" s="18" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Z82" s="18" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AA82" s="18" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="AB82" s="18" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="AC82" s="18" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AD82" s="18" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="AE82" s="18" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AF82" s="18" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AG82" s="18" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AH82" s="18" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="AI82" s="18" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="AJ82" s="18" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="AK82" s="18" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AL82" s="18" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="83" spans="1:38" x14ac:dyDescent="0.35">
@@ -7403,112 +7409,112 @@
         <v>75</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D83" s="18" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E83" s="18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F83" s="18" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G83" s="18" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H83" s="18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I83" s="18" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J83" s="18" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K83" s="18" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="L83" s="18" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="M83" s="18" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="N83" s="18" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="O83" s="18" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="P83" s="18" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="Q83" s="18" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="R83" s="18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="S83" s="18" t="s">
+        <v>483</v>
+      </c>
+      <c r="T83" s="18" t="s">
         <v>484</v>
       </c>
-      <c r="T83" s="18" t="s">
-        <v>485</v>
-      </c>
       <c r="U83" s="18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="V83" s="18" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="W83" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="X83" s="18" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Y83" s="18" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Z83" s="18" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="AA83" s="18" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="AB83" s="18" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="AC83" s="18" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="AD83" s="18" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="AE83" s="18" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AF83" s="18" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AG83" s="18" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="AH83" s="18" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="AI83" s="18" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="AJ83" s="18" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="AK83" s="18" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AL83" s="18" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="84" spans="1:38" ht="72.5" x14ac:dyDescent="0.35">
@@ -7517,110 +7523,110 @@
         <v>76</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F84" s="26" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G84" s="26" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H84" s="26" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="J84" s="26" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K84" s="26" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="L84" s="26" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="M84" s="26" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="N84" s="26" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="O84" s="26" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="P84" s="26" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="Q84" s="26" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="R84" s="26" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="S84" s="26" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="T84" s="26" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="U84" s="26" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="V84" s="26" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="W84" s="26" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="X84" s="26" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Y84" s="26" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Z84" s="26" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="AA84" s="26" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="AB84" s="26" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="AC84" s="26" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AD84" s="26"/>
       <c r="AE84" s="26" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AF84" s="26" t="s">
+        <v>540</v>
+      </c>
+      <c r="AG84" s="26" t="s">
         <v>541</v>
       </c>
-      <c r="AG84" s="26" t="s">
-        <v>542</v>
-      </c>
       <c r="AH84" s="26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="AI84" s="26" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="AJ84" s="26" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="AK84" s="26" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AL84" s="26" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct actors type section
</commit_message>
<xml_diff>
--- a/excel-use-cases/MAESHA/IEC62559-2_TEMPLATE_FrequencyControlUC.xlsx
+++ b/excel-use-cases/MAESHA/IEC62559-2_TEMPLATE_FrequencyControlUC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MAESHA\08_BRIDGE\Data Management WG\UC repository\MAESHA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB224ABE-0A52-4710-83E1-48B0AF17912A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60B934E-69E6-469B-98CC-C93923ABBD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1363,7 +1363,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="517">
   <si>
     <t>1 Description of the use case</t>
   </si>
@@ -1701,16 +1701,7 @@
     <t>Physical or legal person that has his own interests, defined as "Business Goals"</t>
   </si>
   <si>
-    <t>Logical actors</t>
-  </si>
-  <si>
     <t>Technical entity that takes part in the execution of a use case. A logical actor can be mapped to a physical component</t>
-  </si>
-  <si>
-    <t>Assets</t>
-  </si>
-  <si>
-    <t>Devices</t>
   </si>
   <si>
     <t>TSO</t>
@@ -4010,8 +4001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W48" sqref="W48"/>
+    <sheetView tabSelected="1" topLeftCell="U36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4116,7 +4107,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -4212,7 +4203,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="58" x14ac:dyDescent="0.35">
@@ -4246,7 +4237,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="409.5" x14ac:dyDescent="0.35">
@@ -4255,7 +4246,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -4332,7 +4323,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="24" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -4344,7 +4335,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="19"/>
@@ -4524,22 +4515,22 @@
         <v>80</v>
       </c>
       <c r="C41" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>495</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="F41" s="18" t="s">
         <v>497</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="G41" s="18" t="s">
         <v>498</v>
       </c>
-      <c r="E41" s="18" t="s">
+      <c r="H41" s="18" t="s">
         <v>499</v>
-      </c>
-      <c r="F41" s="18" t="s">
-        <v>500</v>
-      </c>
-      <c r="G41" s="18" t="s">
-        <v>501</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="42" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -4584,13 +4575,13 @@
         <v>110</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="E44" s="18" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="F44" s="18" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
@@ -4619,7 +4610,7 @@
         <v>111</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E45" s="18"/>
       <c r="F45" s="18"/>
@@ -4647,67 +4638,67 @@
         <v>41</v>
       </c>
       <c r="C46" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D46" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="E46" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="E46" s="18" t="s">
-        <v>122</v>
-      </c>
       <c r="F46" s="18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G46" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H46" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="H46" s="18" t="s">
-        <v>129</v>
-      </c>
       <c r="I46" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K46" s="18" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="L46" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="M46" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="N46" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="O46" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="P46" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q46" s="18" t="s">
         <v>145</v>
       </c>
-      <c r="P46" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q46" s="18" t="s">
-        <v>148</v>
-      </c>
       <c r="R46" s="18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="S46" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="T46" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="U46" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="T46" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="U46" s="18" t="s">
-        <v>155</v>
-      </c>
       <c r="V46" s="18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="W46" s="18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.35">
@@ -4716,67 +4707,67 @@
         <v>42</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F47" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="I47" s="18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="J47" s="18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="K47" s="18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="L47" s="18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="M47" s="18" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="N47" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="O47" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="P47" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="Q47" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="R47" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="S47" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="T47" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="U47" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="V47" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="W47" s="18" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="58" x14ac:dyDescent="0.35">
@@ -4785,67 +4776,67 @@
         <v>43</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E48" s="18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F48" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="G48" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="G48" s="26" t="s">
-        <v>128</v>
-      </c>
       <c r="H48" s="26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="I48" s="26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J48" s="26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="K48" s="26" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="L48" s="26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M48" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="N48" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="N48" s="26" t="s">
-        <v>143</v>
-      </c>
       <c r="O48" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="P48" s="26" t="s">
         <v>144</v>
       </c>
-      <c r="P48" s="26" t="s">
-        <v>147</v>
-      </c>
       <c r="Q48" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="R48" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="S48" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="R48" s="26" t="s">
-        <v>151</v>
-      </c>
-      <c r="S48" s="26" t="s">
-        <v>152</v>
-      </c>
       <c r="T48" s="26" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="U48" s="26" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="V48" s="26" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="W48" s="26" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.35">
@@ -4854,7 +4845,7 @@
         <v>44</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
@@ -4893,13 +4884,13 @@
         <v>21</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E51" s="18" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F51" s="18"/>
     </row>
@@ -4909,13 +4900,13 @@
         <v>46</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F52" s="18"/>
     </row>
@@ -4925,13 +4916,13 @@
         <v>47</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F53" s="18"/>
     </row>
@@ -4941,13 +4932,13 @@
         <v>48</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E54" s="18" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F54" s="18"/>
     </row>
@@ -4963,7 +4954,7 @@
         <v>90</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F55" s="18"/>
     </row>
@@ -4973,13 +4964,13 @@
         <v>50</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E56" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F56" s="18"/>
     </row>
@@ -4989,13 +4980,13 @@
         <v>51</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F57" s="18"/>
     </row>
@@ -5005,13 +4996,13 @@
         <v>52</v>
       </c>
       <c r="C58" s="27" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E58" s="29" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F58" s="18"/>
     </row>
@@ -5049,28 +5040,28 @@
         <v>46</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E62" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G62" s="18" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H62" s="18" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="I62" s="18" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J62" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63" spans="1:23" ht="29" x14ac:dyDescent="0.35">
@@ -5079,28 +5070,28 @@
         <v>56</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E63" s="18" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F63" s="18" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G63" s="18" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="H63" s="26" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I63" s="26" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="J63" s="26" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="64" spans="1:23" ht="29" x14ac:dyDescent="0.35">
@@ -5109,28 +5100,28 @@
         <v>57</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D64" s="26" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E64" s="18" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F64" s="26" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G64" s="26" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="H64" s="26" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="I64" s="26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="J64" s="26" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="65" spans="1:59" x14ac:dyDescent="0.35">
@@ -5139,28 +5130,28 @@
         <v>58</v>
       </c>
       <c r="C65" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D65" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D65" s="18" t="s">
-        <v>119</v>
-      </c>
       <c r="E65" s="18" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="F65" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="G65" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="G65" s="18" t="s">
-        <v>119</v>
-      </c>
       <c r="H65" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="I65" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="J65" s="18" t="s">
         <v>116</v>
-      </c>
-      <c r="J65" s="18" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:59" x14ac:dyDescent="0.35">
@@ -5169,28 +5160,28 @@
         <v>59</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E66" s="18" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F66" s="18" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G66" s="18" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H66" s="18" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="I66" s="18" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:59" ht="29" x14ac:dyDescent="0.35">
@@ -5199,28 +5190,28 @@
         <v>60</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E67" s="18" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F67" s="18" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G67" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H67" s="26" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="I67" s="26" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="J67" s="26" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" spans="1:59" ht="29" x14ac:dyDescent="0.35">
@@ -5229,28 +5220,28 @@
         <v>61</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E68" s="18" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F68" s="26" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G68" s="26" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="H68" s="26" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I68" s="26" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="J68" s="26" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="69" spans="1:59" x14ac:dyDescent="0.35">
@@ -5322,175 +5313,175 @@
         <v>63</v>
       </c>
       <c r="C70" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="F70" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="G70" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="H70" s="18" t="s">
+        <v>500</v>
+      </c>
+      <c r="I70" s="26" t="s">
+        <v>501</v>
+      </c>
+      <c r="J70" s="26" t="s">
+        <v>501</v>
+      </c>
+      <c r="K70" s="26" t="s">
+        <v>501</v>
+      </c>
+      <c r="L70" s="26" t="s">
+        <v>502</v>
+      </c>
+      <c r="M70" s="26" t="s">
+        <v>502</v>
+      </c>
+      <c r="N70" s="26" t="s">
+        <v>502</v>
+      </c>
+      <c r="O70" s="26" t="s">
+        <v>502</v>
+      </c>
+      <c r="P70" s="26" t="s">
+        <v>502</v>
+      </c>
+      <c r="Q70" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="R70" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="E70" s="18" t="s">
+      <c r="S70" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="F70" s="18" t="s">
+      <c r="T70" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="G70" s="18" t="s">
+      <c r="U70" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="H70" s="18" t="s">
+      <c r="V70" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="I70" s="26" t="s">
+      <c r="W70" s="26" t="s">
+        <v>503</v>
+      </c>
+      <c r="X70" s="26" t="s">
         <v>504</v>
       </c>
-      <c r="J70" s="26" t="s">
+      <c r="Y70" s="26" t="s">
         <v>504</v>
       </c>
-      <c r="K70" s="26" t="s">
+      <c r="Z70" s="26" t="s">
         <v>504</v>
       </c>
-      <c r="L70" s="26" t="s">
+      <c r="AA70" s="26" t="s">
+        <v>504</v>
+      </c>
+      <c r="AB70" s="26" t="s">
+        <v>504</v>
+      </c>
+      <c r="AC70" s="26" t="s">
+        <v>504</v>
+      </c>
+      <c r="AD70" s="26" t="s">
+        <v>504</v>
+      </c>
+      <c r="AE70" s="26" t="s">
         <v>505</v>
       </c>
-      <c r="M70" s="26" t="s">
+      <c r="AF70" s="26" t="s">
         <v>505</v>
       </c>
-      <c r="N70" s="26" t="s">
+      <c r="AG70" s="26" t="s">
         <v>505</v>
       </c>
-      <c r="O70" s="26" t="s">
+      <c r="AH70" s="26" t="s">
         <v>505</v>
       </c>
-      <c r="P70" s="26" t="s">
+      <c r="AI70" s="26" t="s">
         <v>505</v>
       </c>
-      <c r="Q70" s="26" t="s">
+      <c r="AJ70" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="AK70" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="AL70" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="AM70" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="AN70" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="AO70" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="AP70" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="AQ70" s="26" t="s">
+        <v>505</v>
+      </c>
+      <c r="AR70" s="26" t="s">
         <v>506</v>
       </c>
-      <c r="R70" s="26" t="s">
+      <c r="AS70" s="26" t="s">
         <v>506</v>
       </c>
-      <c r="S70" s="26" t="s">
+      <c r="AT70" s="26" t="s">
         <v>506</v>
       </c>
-      <c r="T70" s="26" t="s">
-        <v>506</v>
-      </c>
-      <c r="U70" s="26" t="s">
-        <v>506</v>
-      </c>
-      <c r="V70" s="26" t="s">
-        <v>506</v>
-      </c>
-      <c r="W70" s="26" t="s">
-        <v>506</v>
-      </c>
-      <c r="X70" s="26" t="s">
+      <c r="AU70" s="26" t="s">
         <v>507</v>
       </c>
-      <c r="Y70" s="26" t="s">
+      <c r="AV70" s="26" t="s">
         <v>507</v>
       </c>
-      <c r="Z70" s="26" t="s">
+      <c r="AW70" s="26" t="s">
         <v>507</v>
       </c>
-      <c r="AA70" s="26" t="s">
+      <c r="AX70" s="26" t="s">
         <v>507</v>
       </c>
-      <c r="AB70" s="26" t="s">
+      <c r="AY70" s="26" t="s">
         <v>507</v>
       </c>
-      <c r="AC70" s="26" t="s">
+      <c r="AZ70" s="26" t="s">
         <v>507</v>
       </c>
-      <c r="AD70" s="26" t="s">
+      <c r="BA70" s="26" t="s">
         <v>507</v>
       </c>
-      <c r="AE70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AF70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AG70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AH70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AI70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AJ70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AK70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AL70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AM70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AN70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AO70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AP70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AQ70" s="26" t="s">
-        <v>508</v>
-      </c>
-      <c r="AR70" s="26" t="s">
-        <v>509</v>
-      </c>
-      <c r="AS70" s="26" t="s">
-        <v>509</v>
-      </c>
-      <c r="AT70" s="26" t="s">
-        <v>509</v>
-      </c>
-      <c r="AU70" s="26" t="s">
-        <v>510</v>
-      </c>
-      <c r="AV70" s="26" t="s">
-        <v>510</v>
-      </c>
-      <c r="AW70" s="26" t="s">
-        <v>510</v>
-      </c>
-      <c r="AX70" s="26" t="s">
-        <v>510</v>
-      </c>
-      <c r="AY70" s="26" t="s">
-        <v>510</v>
-      </c>
-      <c r="AZ70" s="26" t="s">
-        <v>510</v>
-      </c>
-      <c r="BA70" s="26" t="s">
-        <v>510</v>
-      </c>
       <c r="BB70" s="26" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="BC70" s="26" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="BD70" s="26" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="BE70" s="26" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="BF70" s="26" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="BG70" s="26" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="71" spans="1:59" x14ac:dyDescent="0.35">
@@ -5589,10 +5580,10 @@
         <v>2</v>
       </c>
       <c r="AG71" s="18" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="AH71" s="18" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="AI71" s="18">
         <v>4</v>
@@ -5610,10 +5601,10 @@
         <v>8</v>
       </c>
       <c r="AN71" s="18" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="AO71" s="18" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="AP71" s="18">
         <v>10</v>
@@ -5676,175 +5667,175 @@
         <v>65</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="E72" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="F72" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="G72" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H72" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="I72" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="I72" s="26" t="s">
+      <c r="J72" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="J72" s="26" t="s">
+      <c r="K72" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="K72" s="26" t="s">
+      <c r="L72" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="L72" s="26" t="s">
-        <v>250</v>
-      </c>
       <c r="M72" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N72" s="26" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="O72" s="26" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="P72" s="26" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="Q72" s="26" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="R72" s="26" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="S72" s="26" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="T72" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="U72" s="26" t="s">
         <v>278</v>
       </c>
-      <c r="U72" s="26" t="s">
+      <c r="V72" s="26" t="s">
         <v>281</v>
       </c>
-      <c r="V72" s="26" t="s">
+      <c r="W72" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="W72" s="26" t="s">
+      <c r="X72" s="26" t="s">
         <v>287</v>
       </c>
-      <c r="X72" s="26" t="s">
+      <c r="Y72" s="26" t="s">
         <v>290</v>
       </c>
-      <c r="Y72" s="26" t="s">
+      <c r="Z72" s="26" t="s">
         <v>293</v>
       </c>
-      <c r="Z72" s="26" t="s">
+      <c r="AA72" s="26" t="s">
         <v>296</v>
       </c>
-      <c r="AA72" s="26" t="s">
-        <v>299</v>
-      </c>
       <c r="AB72" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AC72" s="26" t="s">
+        <v>301</v>
+      </c>
+      <c r="AD72" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="AD72" s="26" t="s">
+      <c r="AE72" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="AE72" s="26" t="s">
+      <c r="AF72" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="AF72" s="26" t="s">
+      <c r="AG72" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="AG72" s="26" t="s">
+      <c r="AH72" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="AH72" s="26" t="s">
+      <c r="AI72" s="26" t="s">
         <v>319</v>
       </c>
-      <c r="AI72" s="26" t="s">
+      <c r="AJ72" s="26" t="s">
         <v>322</v>
       </c>
-      <c r="AJ72" s="26" t="s">
+      <c r="AK72" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="AK72" s="26" t="s">
-        <v>328</v>
-      </c>
       <c r="AL72" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AM72" s="26" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="AN72" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="AO72" s="26" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="AP72" s="26" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="AQ72" s="26" t="s">
+        <v>338</v>
+      </c>
+      <c r="AR72" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="AR72" s="26" t="s">
+      <c r="AS72" s="26" t="s">
         <v>344</v>
       </c>
-      <c r="AS72" s="26" t="s">
+      <c r="AT72" s="26" t="s">
         <v>347</v>
       </c>
-      <c r="AT72" s="26" t="s">
-        <v>350</v>
-      </c>
       <c r="AU72" s="26" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="AV72" s="26" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="AW72" s="26" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="AX72" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="AY72" s="26" t="s">
         <v>360</v>
       </c>
-      <c r="AY72" s="26" t="s">
-        <v>363</v>
-      </c>
       <c r="AZ72" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="BA72" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="BB72" s="26" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="BC72" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="BD72" s="26" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="BE72" s="26" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="BF72" s="26" t="s">
+        <v>375</v>
+      </c>
+      <c r="BG72" s="26" t="s">
         <v>378</v>
-      </c>
-      <c r="BG72" s="26" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="73" spans="1:59" ht="29" x14ac:dyDescent="0.35">
@@ -5853,175 +5844,175 @@
         <v>66</v>
       </c>
       <c r="C73" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="D73" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="D73" s="18" t="s">
+      <c r="E73" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="E73" s="18" t="s">
-        <v>232</v>
-      </c>
       <c r="F73" s="18" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G73" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="H73" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="H73" s="18" t="s">
+      <c r="I73" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="I73" s="18" t="s">
+      <c r="J73" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="J73" s="26" t="s">
+      <c r="K73" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="K73" s="18" t="s">
+      <c r="L73" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="L73" s="18" t="s">
-        <v>251</v>
-      </c>
       <c r="M73" s="18" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N73" s="26" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="O73" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="P73" s="26" t="s">
         <v>259</v>
       </c>
-      <c r="P73" s="26" t="s">
-        <v>262</v>
-      </c>
       <c r="Q73" s="26" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="R73" s="26" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="S73" s="26" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="T73" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="U73" s="26" t="s">
         <v>279</v>
       </c>
-      <c r="U73" s="26" t="s">
+      <c r="V73" s="26" t="s">
         <v>282</v>
       </c>
-      <c r="V73" s="26" t="s">
+      <c r="W73" s="26" t="s">
         <v>285</v>
       </c>
-      <c r="W73" s="26" t="s">
+      <c r="X73" s="26" t="s">
         <v>288</v>
       </c>
-      <c r="X73" s="26" t="s">
+      <c r="Y73" s="26" t="s">
         <v>291</v>
       </c>
-      <c r="Y73" s="26" t="s">
+      <c r="Z73" s="26" t="s">
         <v>294</v>
       </c>
-      <c r="Z73" s="26" t="s">
+      <c r="AA73" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="AA73" s="26" t="s">
-        <v>300</v>
-      </c>
       <c r="AB73" s="26" t="s">
+        <v>299</v>
+      </c>
+      <c r="AC73" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="AC73" s="26" t="s">
+      <c r="AD73" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="AD73" s="26" t="s">
+      <c r="AE73" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="AE73" s="26" t="s">
+      <c r="AF73" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="AF73" s="26" t="s">
+      <c r="AG73" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="AG73" s="26" t="s">
+      <c r="AH73" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="AH73" s="26" t="s">
+      <c r="AI73" s="26" t="s">
         <v>320</v>
       </c>
-      <c r="AI73" s="26" t="s">
+      <c r="AJ73" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="AJ73" s="26" t="s">
-        <v>326</v>
-      </c>
       <c r="AK73" s="26" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AL73" s="26" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="AM73" s="26" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="AN73" s="26" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AO73" s="26" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="AP73" s="26" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="AQ73" s="26" t="s">
+        <v>339</v>
+      </c>
+      <c r="AR73" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="AR73" s="26" t="s">
+      <c r="AS73" s="26" t="s">
         <v>345</v>
       </c>
-      <c r="AS73" s="26" t="s">
+      <c r="AT73" s="26" t="s">
         <v>348</v>
       </c>
-      <c r="AT73" s="26" t="s">
-        <v>351</v>
-      </c>
       <c r="AU73" s="26" t="s">
+        <v>350</v>
+      </c>
+      <c r="AV73" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="AV73" s="26" t="s">
-        <v>356</v>
-      </c>
       <c r="AW73" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="AX73" s="26" t="s">
         <v>358</v>
       </c>
-      <c r="AX73" s="26" t="s">
+      <c r="AY73" s="26" t="s">
         <v>361</v>
       </c>
-      <c r="AY73" s="26" t="s">
-        <v>364</v>
-      </c>
       <c r="AZ73" s="26" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="BA73" s="26" t="s">
+        <v>365</v>
+      </c>
+      <c r="BB73" s="26" t="s">
         <v>368</v>
       </c>
-      <c r="BB73" s="26" t="s">
-        <v>371</v>
-      </c>
       <c r="BC73" s="26" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="BD73" s="26" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="BE73" s="26" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="BF73" s="26" t="s">
+        <v>376</v>
+      </c>
+      <c r="BG73" s="26" t="s">
         <v>379</v>
-      </c>
-      <c r="BG73" s="26" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="74" spans="1:59" ht="130.5" x14ac:dyDescent="0.35">
@@ -6030,175 +6021,175 @@
         <v>67</v>
       </c>
       <c r="C74" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D74" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="D74" s="26" t="s">
+      <c r="E74" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="E74" s="26" t="s">
-        <v>233</v>
-      </c>
       <c r="F74" s="26" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G74" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="H74" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="H74" s="26" t="s">
+      <c r="I74" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="I74" s="26" t="s">
+      <c r="J74" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="J74" s="26" t="s">
+      <c r="K74" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="K74" s="26" t="s">
+      <c r="L74" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="L74" s="26" t="s">
-        <v>252</v>
-      </c>
       <c r="M74" s="26" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="N74" s="26" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="O74" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="P74" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="P74" s="26" t="s">
-        <v>263</v>
-      </c>
       <c r="Q74" s="26" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="R74" s="26" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="S74" s="26" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="T74" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="U74" s="26" t="s">
         <v>280</v>
       </c>
-      <c r="U74" s="26" t="s">
+      <c r="V74" s="26" t="s">
         <v>283</v>
       </c>
-      <c r="V74" s="26" t="s">
+      <c r="W74" s="26" t="s">
         <v>286</v>
       </c>
-      <c r="W74" s="26" t="s">
+      <c r="X74" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="X74" s="26" t="s">
+      <c r="Y74" s="26" t="s">
         <v>292</v>
       </c>
-      <c r="Y74" s="26" t="s">
+      <c r="Z74" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="Z74" s="26" t="s">
+      <c r="AA74" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="AA74" s="26" t="s">
-        <v>301</v>
-      </c>
       <c r="AB74" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="AC74" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="AC74" s="26" t="s">
+      <c r="AD74" s="26" t="s">
         <v>306</v>
       </c>
-      <c r="AD74" s="26" t="s">
+      <c r="AE74" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="AE74" s="26" t="s">
+      <c r="AF74" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="AF74" s="26" t="s">
+      <c r="AG74" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="AG74" s="26" t="s">
+      <c r="AH74" s="26" t="s">
         <v>318</v>
       </c>
-      <c r="AH74" s="26" t="s">
+      <c r="AI74" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="AI74" s="26" t="s">
+      <c r="AJ74" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="AJ74" s="26" t="s">
-        <v>327</v>
-      </c>
       <c r="AK74" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="AL74" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="AL74" s="26" t="s">
-        <v>332</v>
-      </c>
       <c r="AM74" s="26" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="AN74" s="26" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="AO74" s="26" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="AP74" s="26" t="s">
+        <v>337</v>
+      </c>
+      <c r="AQ74" s="26" t="s">
         <v>340</v>
       </c>
-      <c r="AQ74" s="26" t="s">
+      <c r="AR74" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="AR74" s="26" t="s">
+      <c r="AS74" s="26" t="s">
         <v>346</v>
       </c>
-      <c r="AS74" s="26" t="s">
+      <c r="AT74" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="AT74" s="26" t="s">
-        <v>352</v>
-      </c>
       <c r="AU74" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="AV74" s="26" t="s">
         <v>354</v>
       </c>
-      <c r="AV74" s="26" t="s">
-        <v>357</v>
-      </c>
       <c r="AW74" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="AX74" s="26" t="s">
         <v>359</v>
       </c>
-      <c r="AX74" s="26" t="s">
+      <c r="AY74" s="26" t="s">
         <v>362</v>
       </c>
-      <c r="AY74" s="26" t="s">
-        <v>365</v>
-      </c>
       <c r="AZ74" s="26" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="BA74" s="26" t="s">
+        <v>366</v>
+      </c>
+      <c r="BB74" s="26" t="s">
         <v>369</v>
       </c>
-      <c r="BB74" s="26" t="s">
-        <v>372</v>
-      </c>
       <c r="BC74" s="26" t="s">
+        <v>370</v>
+      </c>
+      <c r="BD74" s="26" t="s">
         <v>373</v>
       </c>
-      <c r="BD74" s="26" t="s">
-        <v>376</v>
-      </c>
       <c r="BE74" s="26" t="s">
+        <v>374</v>
+      </c>
+      <c r="BF74" s="26" t="s">
         <v>377</v>
       </c>
-      <c r="BF74" s="26" t="s">
+      <c r="BG74" s="26" t="s">
         <v>380</v>
-      </c>
-      <c r="BG74" s="26" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="75" spans="1:59" x14ac:dyDescent="0.35">
@@ -6207,175 +6198,175 @@
         <v>68</v>
       </c>
       <c r="C75" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="D75" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="D75" s="18" t="s">
-        <v>231</v>
-      </c>
       <c r="E75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="F75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="G75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="H75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="I75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="J75" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="F75" s="18" t="s">
+      <c r="K75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="L75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="M75" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="G75" s="18" t="s">
+      <c r="N75" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="O75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="P75" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="R75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="S75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="T75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="U75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="V75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="W75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="X75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="Z75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AA75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AB75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC75" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="AD75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AE75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AF75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG75" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="H75" s="18" t="s">
+      <c r="AH75" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="I75" s="18" t="s">
+      <c r="AI75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AJ75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AK75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AL75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AM75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AN75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AO75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AP75" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="AQ75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AR75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AS75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AU75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AV75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AW75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="AY75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="AZ75" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA75" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="J75" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="K75" s="18" t="s">
+      <c r="BB75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="BC75" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="L75" s="18" t="s">
+      <c r="BD75" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="BE75" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="M75" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="N75" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="O75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="P75" s="18" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="R75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="S75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="T75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="U75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="V75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="W75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="X75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="Y75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="Z75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AA75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AB75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AC75" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="AD75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AE75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AF75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AG75" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="AH75" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="AI75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AJ75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AK75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AL75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AM75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AN75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AO75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AP75" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="AQ75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AR75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AS75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AT75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AU75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AV75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AW75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AX75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="AY75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="AZ75" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="BA75" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="BB75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="BC75" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="BD75" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="BE75" s="18" t="s">
-        <v>231</v>
-      </c>
       <c r="BF75" s="18" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="BG75" s="18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:59" x14ac:dyDescent="0.35">
@@ -6384,175 +6375,175 @@
         <v>69</v>
       </c>
       <c r="C76" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="F76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="G76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="H76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="I76" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="J76" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="K76" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="L76" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="M76" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="N76" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="O76" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="P76" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="R76" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D76" s="18" t="s">
+      <c r="S76" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="T76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="U76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="V76" s="18" t="s">
+        <v>515</v>
+      </c>
+      <c r="W76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="X76" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y76" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z76" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA76" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="AB76" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD76" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="E76" s="18" t="s">
+      <c r="AE76" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="AF76" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG76" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="AH76" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="AI76" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ76" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK76" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="AL76" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="AM76" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="AN76" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP76" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="AQ76" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="F76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="G76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="H76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="I76" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="J76" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="K76" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="L76" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="M76" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="N76" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="O76" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="P76" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="Q76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="R76" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="S76" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="T76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="U76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="V76" s="18" t="s">
-        <v>518</v>
-      </c>
-      <c r="W76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="X76" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="Y76" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z76" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="AA76" s="18" t="s">
-        <v>512</v>
-      </c>
-      <c r="AB76" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="AD76" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="AE76" s="18" t="s">
-        <v>513</v>
-      </c>
-      <c r="AF76" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="AG76" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="AH76" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="AI76" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="AJ76" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="AK76" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="AL76" s="18" t="s">
-        <v>512</v>
-      </c>
-      <c r="AM76" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="AN76" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="AO76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="AP76" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="AQ76" s="18" t="s">
-        <v>119</v>
-      </c>
       <c r="AR76" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AS76" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AT76" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AU76" s="18" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="AV76" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="AW76" s="18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AX76" s="18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AY76" s="18" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="AZ76" s="18" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="BA76" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="BB76" s="18" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="BC76" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="BD76" s="18" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="BE76" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="BF76" s="18" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="BG76" s="18" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="77" spans="1:59" x14ac:dyDescent="0.35">
@@ -6624,175 +6615,175 @@
         <v>71</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="D78" s="26" t="s">
+        <v>508</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>393</v>
+      </c>
+      <c r="F78" s="18" t="s">
+        <v>396</v>
+      </c>
+      <c r="G78" s="18" t="s">
+        <v>399</v>
+      </c>
+      <c r="H78" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="I78" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="J78" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="K78" s="18" t="s">
+        <v>407</v>
+      </c>
+      <c r="L78" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="M78" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="N78" s="18" t="s">
+        <v>411</v>
+      </c>
+      <c r="O78" s="18" t="s">
+        <v>413</v>
+      </c>
+      <c r="P78" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="Q78" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="R78" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="S78" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="T78" s="18" t="s">
+        <v>426</v>
+      </c>
+      <c r="U78" s="26" t="s">
+        <v>428</v>
+      </c>
+      <c r="V78" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="W78" s="18" t="s">
+        <v>435</v>
+      </c>
+      <c r="X78" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="Y78" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="Z78" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="AA78" s="18" t="s">
+        <v>443</v>
+      </c>
+      <c r="AB78" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC78" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="AD78" s="18" t="s">
+        <v>446</v>
+      </c>
+      <c r="AE78" s="18" t="s">
+        <v>449</v>
+      </c>
+      <c r="AF78" s="26" t="s">
         <v>511</v>
       </c>
-      <c r="E78" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="F78" s="18" t="s">
-        <v>399</v>
-      </c>
-      <c r="G78" s="18" t="s">
-        <v>402</v>
-      </c>
-      <c r="H78" s="26" t="s">
-        <v>268</v>
-      </c>
-      <c r="I78" s="18" t="s">
-        <v>407</v>
-      </c>
-      <c r="J78" s="18" t="s">
-        <v>407</v>
-      </c>
-      <c r="K78" s="18" t="s">
-        <v>410</v>
-      </c>
-      <c r="L78" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="M78" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="N78" s="18" t="s">
-        <v>414</v>
-      </c>
-      <c r="O78" s="18" t="s">
-        <v>416</v>
-      </c>
-      <c r="P78" s="18" t="s">
-        <v>418</v>
-      </c>
-      <c r="Q78" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="R78" s="18" t="s">
-        <v>423</v>
-      </c>
-      <c r="S78" s="26" t="s">
-        <v>425</v>
-      </c>
-      <c r="T78" s="18" t="s">
-        <v>429</v>
-      </c>
-      <c r="U78" s="26" t="s">
-        <v>431</v>
-      </c>
-      <c r="V78" s="18" t="s">
-        <v>435</v>
-      </c>
-      <c r="W78" s="18" t="s">
-        <v>438</v>
-      </c>
-      <c r="X78" s="18" t="s">
-        <v>441</v>
-      </c>
-      <c r="Y78" s="18" t="s">
-        <v>443</v>
-      </c>
-      <c r="Z78" s="18" t="s">
-        <v>443</v>
-      </c>
-      <c r="AA78" s="18" t="s">
-        <v>446</v>
-      </c>
-      <c r="AB78" s="18" t="s">
-        <v>449</v>
-      </c>
-      <c r="AC78" s="18" t="s">
-        <v>449</v>
-      </c>
-      <c r="AD78" s="18" t="s">
-        <v>449</v>
-      </c>
-      <c r="AE78" s="18" t="s">
+      <c r="AG78" s="18" t="s">
         <v>452</v>
       </c>
-      <c r="AF78" s="26" t="s">
-        <v>514</v>
-      </c>
-      <c r="AG78" s="18" t="s">
+      <c r="AH78" s="18" t="s">
         <v>455</v>
       </c>
-      <c r="AH78" s="18" t="s">
+      <c r="AI78" s="18" t="s">
         <v>458</v>
       </c>
-      <c r="AI78" s="18" t="s">
-        <v>461</v>
-      </c>
       <c r="AJ78" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="AK78" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="AL78" s="26" t="s">
         <v>463</v>
       </c>
-      <c r="AK78" s="26" t="s">
+      <c r="AM78" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="AN78" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="AO78" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="AP78" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="AQ78" s="26" t="s">
+        <v>512</v>
+      </c>
+      <c r="AR78" s="26" t="s">
+        <v>513</v>
+      </c>
+      <c r="AS78" s="26" t="s">
+        <v>467</v>
+      </c>
+      <c r="AT78" s="26" t="s">
+        <v>470</v>
+      </c>
+      <c r="AU78" s="26" t="s">
+        <v>473</v>
+      </c>
+      <c r="AV78" s="26" t="s">
+        <v>476</v>
+      </c>
+      <c r="AW78" s="26" t="s">
+        <v>432</v>
+      </c>
+      <c r="AX78" s="26" t="s">
+        <v>476</v>
+      </c>
+      <c r="AY78" s="26" t="s">
+        <v>476</v>
+      </c>
+      <c r="AZ78" s="26" t="s">
+        <v>479</v>
+      </c>
+      <c r="BA78" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="BB78" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="BC78" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="BD78" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="BE78" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="BF78" s="26" t="s">
+        <v>460</v>
+      </c>
+      <c r="BG78" s="26" t="s">
         <v>463</v>
-      </c>
-      <c r="AL78" s="26" t="s">
-        <v>466</v>
-      </c>
-      <c r="AM78" s="26" t="s">
-        <v>468</v>
-      </c>
-      <c r="AN78" s="26" t="s">
-        <v>515</v>
-      </c>
-      <c r="AO78" s="26" t="s">
-        <v>515</v>
-      </c>
-      <c r="AP78" s="26" t="s">
-        <v>515</v>
-      </c>
-      <c r="AQ78" s="26" t="s">
-        <v>515</v>
-      </c>
-      <c r="AR78" s="26" t="s">
-        <v>516</v>
-      </c>
-      <c r="AS78" s="26" t="s">
-        <v>470</v>
-      </c>
-      <c r="AT78" s="26" t="s">
-        <v>473</v>
-      </c>
-      <c r="AU78" s="26" t="s">
-        <v>476</v>
-      </c>
-      <c r="AV78" s="26" t="s">
-        <v>479</v>
-      </c>
-      <c r="AW78" s="26" t="s">
-        <v>435</v>
-      </c>
-      <c r="AX78" s="26" t="s">
-        <v>479</v>
-      </c>
-      <c r="AY78" s="26" t="s">
-        <v>479</v>
-      </c>
-      <c r="AZ78" s="26" t="s">
-        <v>482</v>
-      </c>
-      <c r="BA78" s="26" t="s">
-        <v>463</v>
-      </c>
-      <c r="BB78" s="26" t="s">
-        <v>463</v>
-      </c>
-      <c r="BC78" s="26" t="s">
-        <v>463</v>
-      </c>
-      <c r="BD78" s="26" t="s">
-        <v>463</v>
-      </c>
-      <c r="BE78" s="26" t="s">
-        <v>463</v>
-      </c>
-      <c r="BF78" s="26" t="s">
-        <v>463</v>
-      </c>
-      <c r="BG78" s="26" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="79" spans="1:59" x14ac:dyDescent="0.35">
@@ -6801,175 +6792,175 @@
         <v>77</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E79" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F79" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G79" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="H79" s="18" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="I79" s="18" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="J79" s="18" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="K79" s="18" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L79" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="M79" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="N79" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="O79" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="P79" s="18" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="Q79" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="R79" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="S79" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="T79" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="U79" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="V79" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="W79" s="26" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="X79" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="Y79" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="Z79" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AA79" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AB79" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AC79" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AD79" s="26" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="AE79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AF79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AG79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AH79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AI79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AJ79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AK79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AL79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AM79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AN79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AO79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AP79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AQ79" s="26" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AR79" s="26" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AS79" s="26" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AT79" s="26" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AU79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AV79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AW79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AX79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AY79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="AZ79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="BA79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="BB79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="BC79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="BD79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="BE79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="BF79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="BG79" s="26" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="80" spans="1:59" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -7061,112 +7052,112 @@
         <v>74</v>
       </c>
       <c r="C82" s="7" t="s">
+        <v>381</v>
+      </c>
+      <c r="D82" s="18" t="s">
         <v>384</v>
       </c>
-      <c r="D82" s="18" t="s">
+      <c r="E82" s="18" t="s">
         <v>387</v>
       </c>
-      <c r="E82" s="18" t="s">
+      <c r="F82" s="18" t="s">
         <v>390</v>
       </c>
-      <c r="F82" s="18" t="s">
+      <c r="G82" s="18" t="s">
         <v>393</v>
       </c>
-      <c r="G82" s="18" t="s">
+      <c r="H82" s="18" t="s">
         <v>396</v>
       </c>
-      <c r="H82" s="18" t="s">
+      <c r="I82" s="18" t="s">
         <v>399</v>
       </c>
-      <c r="I82" s="18" t="s">
-        <v>402</v>
-      </c>
       <c r="J82" s="18" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="K82" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="L82" s="18" t="s">
         <v>407</v>
       </c>
-      <c r="L82" s="18" t="s">
-        <v>410</v>
-      </c>
       <c r="M82" s="18" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="N82" s="18" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="O82" s="18" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="P82" s="18" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="Q82" s="18" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="R82" s="18" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="S82" s="18" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="T82" s="18" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="U82" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="V82" s="18" t="s">
         <v>435</v>
       </c>
-      <c r="V82" s="18" t="s">
+      <c r="W82" s="18" t="s">
         <v>438</v>
       </c>
-      <c r="W82" s="18" t="s">
-        <v>441</v>
-      </c>
       <c r="X82" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="Y82" s="18" t="s">
         <v>443</v>
       </c>
-      <c r="Y82" s="18" t="s">
+      <c r="Z82" s="18" t="s">
         <v>446</v>
       </c>
-      <c r="Z82" s="18" t="s">
+      <c r="AA82" s="18" t="s">
         <v>449</v>
       </c>
-      <c r="AA82" s="18" t="s">
+      <c r="AB82" s="18" t="s">
         <v>452</v>
       </c>
-      <c r="AB82" s="18" t="s">
+      <c r="AC82" s="18" t="s">
         <v>455</v>
       </c>
-      <c r="AC82" s="18" t="s">
+      <c r="AD82" s="18" t="s">
         <v>458</v>
       </c>
-      <c r="AD82" s="18" t="s">
-        <v>461</v>
-      </c>
       <c r="AE82" s="18" t="s">
+        <v>460</v>
+      </c>
+      <c r="AF82" s="18" t="s">
         <v>463</v>
       </c>
-      <c r="AF82" s="18" t="s">
-        <v>466</v>
-      </c>
       <c r="AG82" s="18" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="AH82" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="AI82" s="18" t="s">
         <v>470</v>
       </c>
-      <c r="AI82" s="18" t="s">
+      <c r="AJ82" s="18" t="s">
         <v>473</v>
       </c>
-      <c r="AJ82" s="18" t="s">
+      <c r="AK82" s="18" t="s">
         <v>476</v>
       </c>
-      <c r="AK82" s="18" t="s">
+      <c r="AL82" s="18" t="s">
         <v>479</v>
-      </c>
-      <c r="AL82" s="18" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="83" spans="1:38" x14ac:dyDescent="0.35">
@@ -7175,112 +7166,112 @@
         <v>75</v>
       </c>
       <c r="C83" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D83" s="18" t="s">
         <v>385</v>
       </c>
-      <c r="D83" s="18" t="s">
+      <c r="E83" s="18" t="s">
         <v>388</v>
       </c>
-      <c r="E83" s="18" t="s">
+      <c r="F83" s="18" t="s">
         <v>391</v>
       </c>
-      <c r="F83" s="18" t="s">
+      <c r="G83" s="18" t="s">
         <v>394</v>
       </c>
-      <c r="G83" s="18" t="s">
+      <c r="H83" s="18" t="s">
         <v>397</v>
       </c>
-      <c r="H83" s="18" t="s">
+      <c r="I83" s="18" t="s">
         <v>400</v>
       </c>
-      <c r="I83" s="18" t="s">
-        <v>403</v>
-      </c>
       <c r="J83" s="18" t="s">
+        <v>402</v>
+      </c>
+      <c r="K83" s="18" t="s">
         <v>405</v>
       </c>
-      <c r="K83" s="18" t="s">
+      <c r="L83" s="18" t="s">
         <v>408</v>
       </c>
-      <c r="L83" s="18" t="s">
-        <v>411</v>
-      </c>
       <c r="M83" s="18" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="N83" s="18" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="O83" s="18" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="P83" s="18" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="Q83" s="18" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="R83" s="18" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="S83" s="18" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="T83" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="U83" s="18" t="s">
         <v>433</v>
       </c>
-      <c r="U83" s="18" t="s">
+      <c r="V83" s="18" t="s">
         <v>436</v>
       </c>
-      <c r="V83" s="18" t="s">
-        <v>439</v>
-      </c>
       <c r="W83" s="18" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="X83" s="18" t="s">
+        <v>441</v>
+      </c>
+      <c r="Y83" s="18" t="s">
         <v>444</v>
       </c>
-      <c r="Y83" s="18" t="s">
+      <c r="Z83" s="18" t="s">
         <v>447</v>
       </c>
-      <c r="Z83" s="18" t="s">
+      <c r="AA83" s="18" t="s">
         <v>450</v>
       </c>
-      <c r="AA83" s="18" t="s">
+      <c r="AB83" s="18" t="s">
         <v>453</v>
       </c>
-      <c r="AB83" s="18" t="s">
+      <c r="AC83" s="18" t="s">
         <v>456</v>
       </c>
-      <c r="AC83" s="18" t="s">
+      <c r="AD83" s="18" t="s">
         <v>459</v>
       </c>
-      <c r="AD83" s="18" t="s">
-        <v>462</v>
-      </c>
       <c r="AE83" s="18" t="s">
+        <v>461</v>
+      </c>
+      <c r="AF83" s="18" t="s">
         <v>464</v>
       </c>
-      <c r="AF83" s="18" t="s">
-        <v>467</v>
-      </c>
       <c r="AG83" s="18" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="AH83" s="18" t="s">
+        <v>468</v>
+      </c>
+      <c r="AI83" s="18" t="s">
         <v>471</v>
       </c>
-      <c r="AI83" s="18" t="s">
+      <c r="AJ83" s="18" t="s">
         <v>474</v>
       </c>
-      <c r="AJ83" s="18" t="s">
+      <c r="AK83" s="18" t="s">
         <v>477</v>
       </c>
-      <c r="AK83" s="18" t="s">
+      <c r="AL83" s="18" t="s">
         <v>480</v>
-      </c>
-      <c r="AL83" s="18" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="84" spans="1:38" ht="72.5" x14ac:dyDescent="0.35">
@@ -7289,110 +7280,110 @@
         <v>76</v>
       </c>
       <c r="C84" s="24" t="s">
+        <v>383</v>
+      </c>
+      <c r="D84" s="18" t="s">
         <v>386</v>
       </c>
-      <c r="D84" s="18" t="s">
+      <c r="E84" s="26" t="s">
         <v>389</v>
       </c>
-      <c r="E84" s="26" t="s">
+      <c r="F84" s="26" t="s">
         <v>392</v>
       </c>
-      <c r="F84" s="26" t="s">
+      <c r="G84" s="26" t="s">
         <v>395</v>
       </c>
-      <c r="G84" s="26" t="s">
+      <c r="H84" s="26" t="s">
         <v>398</v>
       </c>
-      <c r="H84" s="26" t="s">
+      <c r="I84" s="26" t="s">
         <v>401</v>
       </c>
-      <c r="I84" s="26" t="s">
-        <v>404</v>
-      </c>
       <c r="J84" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="K84" s="26" t="s">
         <v>406</v>
       </c>
-      <c r="K84" s="26" t="s">
+      <c r="L84" s="26" t="s">
         <v>409</v>
       </c>
-      <c r="L84" s="26" t="s">
+      <c r="M84" s="26" t="s">
         <v>412</v>
       </c>
-      <c r="M84" s="26" t="s">
-        <v>415</v>
-      </c>
       <c r="N84" s="26" t="s">
+        <v>414</v>
+      </c>
+      <c r="O84" s="26" t="s">
         <v>417</v>
       </c>
-      <c r="O84" s="26" t="s">
-        <v>420</v>
-      </c>
       <c r="P84" s="26" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="Q84" s="26" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="R84" s="26" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="S84" s="26" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="T84" s="26" t="s">
+        <v>431</v>
+      </c>
+      <c r="U84" s="26" t="s">
         <v>434</v>
       </c>
-      <c r="U84" s="26" t="s">
+      <c r="V84" s="26" t="s">
         <v>437</v>
       </c>
-      <c r="V84" s="26" t="s">
-        <v>440</v>
-      </c>
       <c r="W84" s="26" t="s">
+        <v>439</v>
+      </c>
+      <c r="X84" s="26" t="s">
         <v>442</v>
       </c>
-      <c r="X84" s="26" t="s">
+      <c r="Y84" s="26" t="s">
         <v>445</v>
       </c>
-      <c r="Y84" s="26" t="s">
+      <c r="Z84" s="26" t="s">
         <v>448</v>
       </c>
-      <c r="Z84" s="26" t="s">
+      <c r="AA84" s="26" t="s">
         <v>451</v>
       </c>
-      <c r="AA84" s="26" t="s">
+      <c r="AB84" s="26" t="s">
         <v>454</v>
       </c>
-      <c r="AB84" s="26" t="s">
+      <c r="AC84" s="26" t="s">
         <v>457</v>
-      </c>
-      <c r="AC84" s="26" t="s">
-        <v>460</v>
       </c>
       <c r="AD84" s="26"/>
       <c r="AE84" s="26" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="AF84" s="26" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="AG84" s="26" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="AH84" s="26" t="s">
+        <v>469</v>
+      </c>
+      <c r="AI84" s="26" t="s">
         <v>472</v>
       </c>
-      <c r="AI84" s="26" t="s">
+      <c r="AJ84" s="26" t="s">
         <v>475</v>
       </c>
-      <c r="AJ84" s="26" t="s">
+      <c r="AK84" s="26" t="s">
         <v>478</v>
       </c>
-      <c r="AK84" s="26" t="s">
+      <c r="AL84" s="26" t="s">
         <v>481</v>
-      </c>
-      <c r="AL84" s="26" t="s">
-        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>